<commit_message>
Fixes for web.config: * Tried different code to get web.config to work. * Renamed root files that are causing an infinite loop in web.config. * Updated build files, file lists, maps, index.html, and links.
</commit_message>
<xml_diff>
--- a/_build/urlmap/DC-URLmapping.xlsx
+++ b/_build/urlmap/DC-URLmapping.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="340">
   <si>
     <t>DNN8-Requirements.html</t>
   </si>
@@ -813,9 +813,6 @@
     <t>administrators/administrator-references.html</t>
   </si>
   <si>
-    <t>administrators/dnn8-whats-new.html</t>
-  </si>
-  <si>
     <t>administrators/extensions/install-extension.html</t>
   </si>
   <si>
@@ -843,9 +840,6 @@
     <t>administrators/licensing/troubleshooting-licensing.html</t>
   </si>
   <si>
-    <t>administrators/overview-dnn-platform.html</t>
-  </si>
-  <si>
     <t>administrators/requirements.html</t>
   </si>
   <si>
@@ -891,9 +885,6 @@
     <t>designers/designer-references.html</t>
   </si>
   <si>
-    <t>designers/dnn8-whats-new.html</t>
-  </si>
-  <si>
     <t>designers/extensions/dnn-manifest-schema.html</t>
   </si>
   <si>
@@ -912,9 +903,6 @@
     <t>designers/index.html</t>
   </si>
   <si>
-    <t>designers/overview-dnn-platform.html</t>
-  </si>
-  <si>
     <t>designers/requirements.html</t>
   </si>
   <si>
@@ -987,9 +975,6 @@
     <t>developers/developer-references.html</t>
   </si>
   <si>
-    <t>developers/dnn8-whats-new.html</t>
-  </si>
-  <si>
     <t>developers/extensions/dnn-manifest-schema.html</t>
   </si>
   <si>
@@ -1008,9 +993,6 @@
     <t>developers/index.html</t>
   </si>
   <si>
-    <t>developers/overview-dnn-platform.html</t>
-  </si>
-  <si>
     <t>developers/providers.html</t>
   </si>
   <si>
@@ -1033,6 +1015,27 @@
   </si>
   <si>
     <t>developers/setup/set-up-sql.html</t>
+  </si>
+  <si>
+    <t>Problems with infinite loop in web.config rules if the filenames are the same, case-insensitive.</t>
+  </si>
+  <si>
+    <t>administrators/dnn-platform-overview.html</t>
+  </si>
+  <si>
+    <t>administrators/whats-new-dnn8.html</t>
+  </si>
+  <si>
+    <t>designers/whats-new-dnn8.html</t>
+  </si>
+  <si>
+    <t>developers/whats-new-dnn8.html</t>
+  </si>
+  <si>
+    <t>designers/dnn-platform-overview.html</t>
+  </si>
+  <si>
+    <t>developers/dnn-platform-overview.html</t>
   </si>
 </sst>
 </file>
@@ -1390,8 +1393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D107" sqref="B2:D107"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1443,7 +1446,10 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>265</v>
+        <v>335</v>
+      </c>
+      <c r="E3" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1452,15 +1458,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="B4:B16" si="2">CONCATENATE("Rule-",TEXT(A4,"000"))</f>
         <v>Rule-003</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>266</v>
-      </c>
+        <v>334</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -1468,14 +1478,17 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rule-004</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>267</v>
+        <v>274</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>333</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -1485,14 +1498,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rule-005</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1501,12 +1514,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rule-006</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="D7" t="s">
-        <v>269</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -1514,13 +1531,15 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rule-007</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="D8" t="s">
-        <v>270</v>
-      </c>
-      <c r="F8" s="1"/>
+        <v>267</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -1528,11 +1547,11 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rule-008</v>
       </c>
       <c r="D9" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1541,11 +1560,11 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rule-009</v>
       </c>
       <c r="D10" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F10" s="1"/>
     </row>
@@ -1555,13 +1574,12 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rule-010</v>
       </c>
       <c r="D11" t="s">
-        <v>273</v>
-      </c>
-      <c r="F11" s="1"/>
+        <v>270</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -1569,11 +1587,11 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rule-011</v>
       </c>
       <c r="D12" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F12" s="1"/>
     </row>
@@ -1583,14 +1601,11 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rule-012</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="D13" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F13" s="1"/>
     </row>
@@ -1600,14 +1615,11 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rule-013</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="D14" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F14" s="1"/>
     </row>
@@ -1617,14 +1629,14 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rule-014</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F15" s="1"/>
     </row>
@@ -1634,14 +1646,14 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rule-015</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F16" s="1"/>
     </row>
@@ -1658,7 +1670,7 @@
         <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1674,7 +1686,7 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1690,7 +1702,7 @@
         <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1706,7 +1718,7 @@
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1738,7 +1750,7 @@
         <v>Rule-021</v>
       </c>
       <c r="D22" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1754,7 +1766,7 @@
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1770,7 +1782,7 @@
         <v>21</v>
       </c>
       <c r="D24" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1786,7 +1798,7 @@
         <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F25" s="1"/>
     </row>
@@ -1803,7 +1815,7 @@
         <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F26" s="1"/>
     </row>
@@ -1820,7 +1832,7 @@
         <v>25</v>
       </c>
       <c r="D27" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F27" s="1"/>
     </row>
@@ -1837,7 +1849,7 @@
         <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F28" s="1"/>
     </row>
@@ -1851,7 +1863,7 @@
         <v>Rule-028</v>
       </c>
       <c r="D29" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1864,7 +1876,7 @@
         <v>Rule-029</v>
       </c>
       <c r="D30" t="s">
-        <v>291</v>
+        <v>336</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1880,7 +1892,7 @@
         <v>29</v>
       </c>
       <c r="D31" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F31" s="1"/>
     </row>
@@ -1897,7 +1909,7 @@
         <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="F32" s="1"/>
     </row>
@@ -1914,7 +1926,7 @@
         <v>14</v>
       </c>
       <c r="D33" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1930,7 +1942,7 @@
         <v>28</v>
       </c>
       <c r="D34" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1946,7 +1958,7 @@
         <v>20</v>
       </c>
       <c r="D35" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1962,7 +1974,7 @@
         <v>33</v>
       </c>
       <c r="D36" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1975,7 +1987,7 @@
         <v>Rule-036</v>
       </c>
       <c r="D37" t="s">
-        <v>298</v>
+        <v>338</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1988,7 +2000,7 @@
         <v>Rule-037</v>
       </c>
       <c r="D38" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -2004,7 +2016,7 @@
         <v>13</v>
       </c>
       <c r="D39" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -2020,7 +2032,7 @@
         <v>16</v>
       </c>
       <c r="D40" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -2036,7 +2048,7 @@
         <v>17</v>
       </c>
       <c r="D41" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -2052,7 +2064,7 @@
         <v>15</v>
       </c>
       <c r="D42" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -2068,7 +2080,7 @@
         <v>18</v>
       </c>
       <c r="D43" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2084,7 +2096,7 @@
         <v>19</v>
       </c>
       <c r="D44" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -2100,7 +2112,7 @@
         <v>32</v>
       </c>
       <c r="D45" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2135,7 +2147,7 @@
         <v>26</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>234</v>
@@ -2151,7 +2163,7 @@
         <v>Rule-047</v>
       </c>
       <c r="D48" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2167,7 +2179,7 @@
         <v>35</v>
       </c>
       <c r="D49" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2183,7 +2195,7 @@
         <v>38</v>
       </c>
       <c r="D50" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -2199,7 +2211,7 @@
         <v>36</v>
       </c>
       <c r="D51" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -2215,7 +2227,7 @@
         <v>39</v>
       </c>
       <c r="D52" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -2231,7 +2243,7 @@
         <v>37</v>
       </c>
       <c r="D53" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -2247,7 +2259,7 @@
         <v>40</v>
       </c>
       <c r="D54" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="F54" s="1"/>
     </row>
@@ -2264,7 +2276,7 @@
         <v>41</v>
       </c>
       <c r="D55" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="F55" s="1"/>
     </row>
@@ -2281,7 +2293,7 @@
         <v>42</v>
       </c>
       <c r="D56" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="F56" s="1"/>
     </row>
@@ -2298,7 +2310,7 @@
         <v>51</v>
       </c>
       <c r="D57" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2314,7 +2326,7 @@
         <v>52</v>
       </c>
       <c r="D58" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2330,7 +2342,7 @@
         <v>54</v>
       </c>
       <c r="D59" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="F59" s="1"/>
     </row>
@@ -2344,7 +2356,7 @@
         <v>Rule-059</v>
       </c>
       <c r="D60" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="F60" s="1"/>
     </row>
@@ -2358,7 +2370,7 @@
         <v>Rule-060</v>
       </c>
       <c r="D61" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="F61" s="1"/>
     </row>
@@ -2375,7 +2387,7 @@
         <v>53</v>
       </c>
       <c r="D62" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -2388,7 +2400,7 @@
         <v>Rule-062</v>
       </c>
       <c r="D63" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -2401,7 +2413,7 @@
         <v>Rule-063</v>
       </c>
       <c r="D64" t="s">
-        <v>323</v>
+        <v>337</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -2417,7 +2429,7 @@
         <v>56</v>
       </c>
       <c r="D65" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -2433,217 +2445,217 @@
         <v>57</v>
       </c>
       <c r="D66" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <f t="shared" ref="A67:A78" si="2">A66+1</f>
+        <f t="shared" ref="A67:A78" si="3">A66+1</f>
         <v>66</v>
       </c>
       <c r="B67" s="1" t="str">
-        <f t="shared" ref="B67:B107" si="3">CONCATENATE("Rule-",TEXT(A67,"000"))</f>
+        <f t="shared" ref="B67:B107" si="4">CONCATENATE("Rule-",TEXT(A67,"000"))</f>
         <v>Rule-066</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D67" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>67</v>
       </c>
       <c r="B68" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-067</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D68" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>68</v>
       </c>
       <c r="B69" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-068</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D69" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>69</v>
       </c>
       <c r="B70" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-069</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D70" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
       <c r="B71" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-070</v>
       </c>
       <c r="D71" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>71</v>
       </c>
       <c r="B72" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-071</v>
       </c>
       <c r="D72" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>72</v>
       </c>
       <c r="B73" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-072</v>
       </c>
       <c r="D73" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="F73" s="1"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>73</v>
       </c>
       <c r="B74" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-073</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D74" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="F74" s="1"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>74</v>
       </c>
       <c r="B75" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-074</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>46</v>
       </c>
       <c r="D75" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>75</v>
       </c>
       <c r="B76" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-075</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D76" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>76</v>
       </c>
       <c r="B77" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-076</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>45</v>
       </c>
       <c r="D77" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>77</v>
       </c>
       <c r="B78" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-077</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D78" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <f t="shared" ref="A79:A81" si="4">A78+1</f>
+        <f t="shared" ref="A79:A81" si="5">A78+1</f>
         <v>78</v>
       </c>
       <c r="B79" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-078</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D79" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
+        <f t="shared" si="5"/>
+        <v>79</v>
+      </c>
+      <c r="B80" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>79</v>
-      </c>
-      <c r="B80" s="1" t="str">
-        <f t="shared" si="3"/>
         <v>Rule-079</v>
       </c>
       <c r="C80" s="1" t="s">
@@ -2658,11 +2670,11 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
+        <f t="shared" si="5"/>
+        <v>80</v>
+      </c>
+      <c r="B81" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>80</v>
-      </c>
-      <c r="B81" s="1" t="str">
-        <f t="shared" si="3"/>
         <v>Rule-080</v>
       </c>
       <c r="D81" t="s">
@@ -2671,18 +2683,18 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <f t="shared" ref="A82:A107" si="5">A81+1</f>
+        <f t="shared" ref="A82:A107" si="6">A81+1</f>
         <v>81</v>
       </c>
       <c r="B82" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-081</v>
       </c>
       <c r="C82" t="s">
         <v>238</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>224</v>
@@ -2690,18 +2702,18 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>82</v>
       </c>
       <c r="B83" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-082</v>
       </c>
       <c r="C83" t="s">
         <v>251</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>224</v>
@@ -2709,18 +2721,18 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>83</v>
       </c>
       <c r="B84" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-083</v>
       </c>
       <c r="C84" t="s">
         <v>241</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>224</v>
@@ -2728,18 +2740,18 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>84</v>
       </c>
       <c r="B85" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-084</v>
       </c>
       <c r="C85" t="s">
         <v>252</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>224</v>
@@ -2747,18 +2759,18 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>85</v>
       </c>
       <c r="B86" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-085</v>
       </c>
       <c r="C86" t="s">
         <v>242</v>
       </c>
       <c r="D86" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>224</v>
@@ -2766,18 +2778,18 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>86</v>
       </c>
       <c r="B87" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-086</v>
       </c>
       <c r="C87" t="s">
         <v>253</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>224</v>
@@ -2785,18 +2797,18 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>87</v>
       </c>
       <c r="B88" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-087</v>
       </c>
       <c r="C88" t="s">
         <v>243</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>224</v>
@@ -2804,18 +2816,18 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>88</v>
       </c>
       <c r="B89" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-088</v>
       </c>
       <c r="C89" t="s">
         <v>254</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>224</v>
@@ -2823,18 +2835,18 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>89</v>
       </c>
       <c r="B90" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-089</v>
       </c>
       <c r="C90" t="s">
         <v>239</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>224</v>
@@ -2842,18 +2854,18 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>90</v>
       </c>
       <c r="B91" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-090</v>
       </c>
       <c r="C91" t="s">
         <v>255</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>224</v>
@@ -2861,18 +2873,18 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>91</v>
       </c>
       <c r="B92" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-091</v>
       </c>
       <c r="C92" t="s">
         <v>244</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>224</v>
@@ -2880,18 +2892,18 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>92</v>
       </c>
       <c r="B93" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-092</v>
       </c>
       <c r="C93" t="s">
         <v>256</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>224</v>
@@ -2899,18 +2911,18 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>93</v>
       </c>
       <c r="B94" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-093</v>
       </c>
       <c r="C94" t="s">
         <v>245</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>224</v>
@@ -2918,18 +2930,18 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>94</v>
       </c>
       <c r="B95" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-094</v>
       </c>
       <c r="C95" t="s">
         <v>257</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>224</v>
@@ -2937,18 +2949,18 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>95</v>
       </c>
       <c r="B96" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-095</v>
       </c>
       <c r="C96" t="s">
         <v>246</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>224</v>
@@ -2956,18 +2968,18 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>96</v>
       </c>
       <c r="B97" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-096</v>
       </c>
       <c r="C97" t="s">
         <v>258</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>224</v>
@@ -2975,18 +2987,18 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>97</v>
       </c>
       <c r="B98" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-097</v>
       </c>
       <c r="C98" t="s">
         <v>240</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>224</v>
@@ -2994,18 +3006,18 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>98</v>
       </c>
       <c r="B99" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-098</v>
       </c>
       <c r="C99" t="s">
         <v>259</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>224</v>
@@ -3013,18 +3025,18 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>99</v>
       </c>
       <c r="B100" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-099</v>
       </c>
       <c r="C100" t="s">
         <v>247</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>224</v>
@@ -3032,18 +3044,18 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="B101" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-100</v>
       </c>
       <c r="C101" t="s">
         <v>260</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>224</v>
@@ -3051,18 +3063,18 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>101</v>
       </c>
       <c r="B102" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-101</v>
       </c>
       <c r="C102" t="s">
         <v>248</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>224</v>
@@ -3070,18 +3082,18 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>102</v>
       </c>
       <c r="B103" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-102</v>
       </c>
       <c r="C103" t="s">
         <v>261</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>224</v>
@@ -3089,18 +3101,18 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>103</v>
       </c>
       <c r="B104" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-103</v>
       </c>
       <c r="C104" t="s">
         <v>249</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>224</v>
@@ -3108,18 +3120,18 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>104</v>
       </c>
       <c r="B105" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-104</v>
       </c>
       <c r="C105" t="s">
         <v>262</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>224</v>
@@ -3127,18 +3139,18 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>105</v>
       </c>
       <c r="B106" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-105</v>
       </c>
       <c r="C106" t="s">
         <v>250</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>224</v>
@@ -3146,18 +3158,18 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>106</v>
       </c>
       <c r="B107" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Rule-106</v>
       </c>
       <c r="C107" t="s">
         <v>263</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>224</v>

</xml_diff>

<commit_message>
* Updated web.config with new subfolders. * ditamaps: Moved security topics and reltables to security-*.ditamap. Tweaks in navtitle. * bptext: Added boilerplate for Administrator permissions requirement. * about-jwt: Title changes. * security: Added info about AuthN and AuthZ.
</commit_message>
<xml_diff>
--- a/_build/urlmap/DC-URLmapping.xlsx
+++ b/_build/urlmap/DC-URLmapping.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="20160323 old2new" sheetId="2" r:id="rId2"/>
     <sheet name="20160309 old2new" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="358">
   <si>
     <t>DNN8-Requirements.html</t>
   </si>
@@ -1036,12 +1036,66 @@
   </si>
   <si>
     <t>developers/dnn-platform-overview.html</t>
+  </si>
+  <si>
+    <t>administrators/security</t>
+  </si>
+  <si>
+    <t>administrators/security/</t>
+  </si>
+  <si>
+    <t>administrators/security/jwt</t>
+  </si>
+  <si>
+    <t>administrators/security/jwt/</t>
+  </si>
+  <si>
+    <t>administrators/security/roles</t>
+  </si>
+  <si>
+    <t>administrators/security/roles/</t>
+  </si>
+  <si>
+    <t>developers/security</t>
+  </si>
+  <si>
+    <t>developers/security/</t>
+  </si>
+  <si>
+    <t>developers/security/jwt</t>
+  </si>
+  <si>
+    <t>developers/security/jwt/</t>
+  </si>
+  <si>
+    <t>developers/security/roles</t>
+  </si>
+  <si>
+    <t>developers/security/roles/</t>
+  </si>
+  <si>
+    <t>administrators/security/index.html</t>
+  </si>
+  <si>
+    <t>administrators/security/jwt/index.html</t>
+  </si>
+  <si>
+    <t>administrators/security/roles/index.html</t>
+  </si>
+  <si>
+    <t>developers/security/index.html</t>
+  </si>
+  <si>
+    <t>developers/security/jwt/index.html</t>
+  </si>
+  <si>
+    <t>developers/security/roles/index.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1100,6 +1154,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1147,7 +1204,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1182,7 +1239,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1391,10 +1448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F113"/>
+  <dimension ref="A1:F133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D129" sqref="D129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2454,7 +2511,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="str">
-        <f t="shared" ref="B67:B107" si="4">CONCATENATE("Rule-",TEXT(A67,"000"))</f>
+        <f t="shared" ref="B67:B87" si="4">CONCATENATE("Rule-",TEXT(A67,"000"))</f>
         <v>Rule-066</v>
       </c>
       <c r="C67" s="1" t="s">
@@ -2683,7 +2740,7 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <f t="shared" ref="A82:A107" si="6">A81+1</f>
+        <f t="shared" ref="A82:A119" si="6">A81+1</f>
         <v>81</v>
       </c>
       <c r="B82" s="1" t="str">
@@ -2801,109 +2858,109 @@
         <v>87</v>
       </c>
       <c r="B88" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="B88:B119" si="7">CONCATENATE("Rule-",TEXT(A88,"000"))</f>
         <v>Rule-087</v>
       </c>
-      <c r="C88" t="s">
-        <v>243</v>
+      <c r="C88" s="1" t="s">
+        <v>340</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>275</v>
+        <v>352</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <f t="shared" si="6"/>
         <v>88</v>
       </c>
       <c r="B89" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>Rule-088</v>
       </c>
-      <c r="C89" t="s">
-        <v>254</v>
+      <c r="C89" s="1" t="s">
+        <v>341</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>275</v>
+        <v>352</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <f t="shared" si="6"/>
         <v>89</v>
       </c>
       <c r="B90" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>Rule-089</v>
       </c>
-      <c r="C90" t="s">
-        <v>239</v>
+      <c r="C90" s="1" t="s">
+        <v>342</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>294</v>
+        <v>353</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <f t="shared" si="6"/>
         <v>90</v>
       </c>
       <c r="B91" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>Rule-090</v>
       </c>
-      <c r="C91" t="s">
-        <v>255</v>
+      <c r="C91" s="1" t="s">
+        <v>343</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>294</v>
+        <v>353</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <f t="shared" si="6"/>
         <v>91</v>
       </c>
       <c r="B92" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>Rule-091</v>
       </c>
-      <c r="C92" t="s">
-        <v>244</v>
+      <c r="C92" s="1" t="s">
+        <v>344</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>287</v>
+        <v>354</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <f t="shared" si="6"/>
         <v>92</v>
       </c>
       <c r="B93" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>Rule-092</v>
       </c>
-      <c r="C93" t="s">
-        <v>256</v>
+      <c r="C93" s="1" t="s">
+        <v>345</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>287</v>
+        <v>354</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>224</v>
@@ -2915,14 +2972,14 @@
         <v>93</v>
       </c>
       <c r="B94" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>Rule-093</v>
       </c>
       <c r="C94" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>224</v>
@@ -2934,14 +2991,14 @@
         <v>94</v>
       </c>
       <c r="B95" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>Rule-094</v>
       </c>
       <c r="C95" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>224</v>
@@ -2953,14 +3010,14 @@
         <v>95</v>
       </c>
       <c r="B96" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>Rule-095</v>
       </c>
       <c r="C96" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>224</v>
@@ -2972,14 +3029,14 @@
         <v>96</v>
       </c>
       <c r="B97" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>Rule-096</v>
       </c>
       <c r="C97" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>224</v>
@@ -2991,14 +3048,14 @@
         <v>97</v>
       </c>
       <c r="B98" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>Rule-097</v>
       </c>
       <c r="C98" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>324</v>
+        <v>287</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>224</v>
@@ -3010,14 +3067,14 @@
         <v>98</v>
       </c>
       <c r="B99" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>Rule-098</v>
       </c>
       <c r="C99" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>324</v>
+        <v>287</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>224</v>
@@ -3029,14 +3086,14 @@
         <v>99</v>
       </c>
       <c r="B100" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>Rule-099</v>
       </c>
       <c r="C100" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>224</v>
@@ -3048,14 +3105,14 @@
         <v>100</v>
       </c>
       <c r="B101" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>Rule-100</v>
       </c>
       <c r="C101" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>224</v>
@@ -3067,14 +3124,14 @@
         <v>101</v>
       </c>
       <c r="B102" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>Rule-101</v>
       </c>
       <c r="C102" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>224</v>
@@ -3086,14 +3143,14 @@
         <v>102</v>
       </c>
       <c r="B103" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>Rule-102</v>
       </c>
       <c r="C103" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>224</v>
@@ -3105,14 +3162,14 @@
         <v>103</v>
       </c>
       <c r="B104" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>Rule-103</v>
       </c>
       <c r="C104" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>224</v>
@@ -3124,14 +3181,14 @@
         <v>104</v>
       </c>
       <c r="B105" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>Rule-104</v>
       </c>
       <c r="C105" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>224</v>
@@ -3143,14 +3200,14 @@
         <v>105</v>
       </c>
       <c r="B106" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>Rule-105</v>
       </c>
       <c r="C106" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>327</v>
+        <v>304</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>224</v>
@@ -3162,26 +3219,265 @@
         <v>106</v>
       </c>
       <c r="B107" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>Rule-106</v>
       </c>
       <c r="C107" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>327</v>
+        <v>304</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>224</v>
       </c>
     </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
+        <f t="shared" si="6"/>
+        <v>107</v>
+      </c>
+      <c r="B108" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>Rule-107</v>
+      </c>
+      <c r="C108" t="s">
+        <v>248</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <f t="shared" si="6"/>
+        <v>108</v>
+      </c>
+      <c r="B109" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>Rule-108</v>
+      </c>
+      <c r="C109" t="s">
+        <v>261</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <f t="shared" si="6"/>
+        <v>109</v>
+      </c>
+      <c r="B110" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>Rule-109</v>
+      </c>
+      <c r="C110" t="s">
+        <v>249</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <f t="shared" si="6"/>
+        <v>110</v>
+      </c>
+      <c r="B111" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>Rule-110</v>
+      </c>
+      <c r="C111" t="s">
+        <v>262</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
     <row r="112" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
+        <f t="shared" si="6"/>
+        <v>111</v>
+      </c>
+      <c r="B112" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>Rule-111</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>355</v>
+      </c>
       <c r="E112" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
+        <f t="shared" si="6"/>
+        <v>112</v>
+      </c>
+      <c r="B113" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>Rule-112</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <f t="shared" si="6"/>
+        <v>113</v>
+      </c>
+      <c r="B114" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>Rule-113</v>
+      </c>
+      <c r="C114" t="s">
+        <v>348</v>
+      </c>
+      <c r="D114" t="s">
+        <v>356</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <f t="shared" si="6"/>
+        <v>114</v>
+      </c>
+      <c r="B115" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>Rule-114</v>
+      </c>
+      <c r="C115" t="s">
+        <v>349</v>
+      </c>
+      <c r="D115" t="s">
+        <v>356</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="1">
+        <f t="shared" si="6"/>
+        <v>115</v>
+      </c>
+      <c r="B116" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>Rule-115</v>
+      </c>
+      <c r="C116" t="s">
+        <v>350</v>
+      </c>
+      <c r="D116" t="s">
+        <v>357</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="1">
+        <f t="shared" si="6"/>
+        <v>116</v>
+      </c>
+      <c r="B117" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>Rule-116</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="1">
+        <f t="shared" si="6"/>
+        <v>117</v>
+      </c>
+      <c r="B118" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>Rule-117</v>
+      </c>
+      <c r="C118" t="s">
+        <v>250</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
+        <f t="shared" si="6"/>
+        <v>118</v>
+      </c>
+      <c r="B119" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>Rule-118</v>
+      </c>
+      <c r="C119" t="s">
+        <v>263</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="122" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="123" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="124" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="125" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="126" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="127" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="128" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="129" spans="5:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="130" spans="5:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="131" spans="5:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="132" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E132" s="1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="113" spans="5:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E113" s="1" t="s">
+    <row r="133" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E133" s="1" t="s">
         <v>237</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Simplified rules in web.config.
</commit_message>
<xml_diff>
--- a/_build/urlmap/DC-URLmapping.xlsx
+++ b/_build/urlmap/DC-URLmapping.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="358">
   <si>
     <t>DNN8-Requirements.html</t>
   </si>
@@ -771,6 +771,270 @@
     <t>developers/setup</t>
   </si>
   <si>
+    <t>administrators/administrator-references.html</t>
+  </si>
+  <si>
+    <t>administrators/extensions/install-extension.html</t>
+  </si>
+  <si>
+    <t>administrators/glossary.html</t>
+  </si>
+  <si>
+    <t>administrators/index.html</t>
+  </si>
+  <si>
+    <t>administrators/licensing/activate-license-automatically.html</t>
+  </si>
+  <si>
+    <t>administrators/licensing/activate-license-manually.html</t>
+  </si>
+  <si>
+    <t>administrators/licensing/faq-licensing.html</t>
+  </si>
+  <si>
+    <t>administrators/licensing/index.html</t>
+  </si>
+  <si>
+    <t>administrators/licensing/licensing.html</t>
+  </si>
+  <si>
+    <t>administrators/licensing/troubleshooting-licensing.html</t>
+  </si>
+  <si>
+    <t>administrators/requirements.html</t>
+  </si>
+  <si>
+    <t>administrators/setup/index.html</t>
+  </si>
+  <si>
+    <t>administrators/setup/run-installation-wizard.html</t>
+  </si>
+  <si>
+    <t>administrators/setup/set-up-dnn-folder.html</t>
+  </si>
+  <si>
+    <t>administrators/setup/set-up-dnn.html</t>
+  </si>
+  <si>
+    <t>administrators/setup/set-up-iis.html</t>
+  </si>
+  <si>
+    <t>administrators/setup/set-up-sql.html</t>
+  </si>
+  <si>
+    <t>designers/about-themes.html</t>
+  </si>
+  <si>
+    <t>designers/creating-themes/create-container.html</t>
+  </si>
+  <si>
+    <t>designers/creating-themes/create-css.html</t>
+  </si>
+  <si>
+    <t>designers/creating-themes/create-doctype-xml.html</t>
+  </si>
+  <si>
+    <t>designers/creating-themes/create-layout-template.html</t>
+  </si>
+  <si>
+    <t>designers/creating-themes/create-theme.html</t>
+  </si>
+  <si>
+    <t>designers/creating-themes/index.html</t>
+  </si>
+  <si>
+    <t>designers/designer-references.html</t>
+  </si>
+  <si>
+    <t>designers/extensions/dnn-manifest-schema.html</t>
+  </si>
+  <si>
+    <t>designers/extensions/index.html</t>
+  </si>
+  <si>
+    <t>designers/extensions/install-extension.html</t>
+  </si>
+  <si>
+    <t>designers/extensions/pack-extension.html</t>
+  </si>
+  <si>
+    <t>designers/glossary.html</t>
+  </si>
+  <si>
+    <t>designers/index.html</t>
+  </si>
+  <si>
+    <t>designers/requirements.html</t>
+  </si>
+  <si>
+    <t>designers/setup/index.html</t>
+  </si>
+  <si>
+    <t>designers/setup/run-installation-wizard.html</t>
+  </si>
+  <si>
+    <t>designers/setup/set-up-dnn-folder.html</t>
+  </si>
+  <si>
+    <t>designers/setup/set-up-dnn.html</t>
+  </si>
+  <si>
+    <t>designers/setup/set-up-iis.html</t>
+  </si>
+  <si>
+    <t>designers/setup/set-up-sql.html</t>
+  </si>
+  <si>
+    <t>designers/theme-objects.html</t>
+  </si>
+  <si>
+    <t>developers/about-evs.html</t>
+  </si>
+  <si>
+    <t>developers/about-modules/index.html</t>
+  </si>
+  <si>
+    <t>developers/about-modules/module-architecture.html</t>
+  </si>
+  <si>
+    <t>developers/about-modules/module-development.html</t>
+  </si>
+  <si>
+    <t>developers/about-modules/module-features.html</t>
+  </si>
+  <si>
+    <t>developers/about-modules/mvc-module-development.html</t>
+  </si>
+  <si>
+    <t>developers/about-modules/spa-module-development.html</t>
+  </si>
+  <si>
+    <t>developers/about-modules/unsupported-mvc-features.html</t>
+  </si>
+  <si>
+    <t>developers/about-modules/web-forms-module-development.html</t>
+  </si>
+  <si>
+    <t>developers/creating-modules/create-module-using-templates.html</t>
+  </si>
+  <si>
+    <t>developers/creating-modules/create-module.html</t>
+  </si>
+  <si>
+    <t>developers/creating-modules/index.html</t>
+  </si>
+  <si>
+    <t>developers/creating-modules/start-vs-project-with-templates.html</t>
+  </si>
+  <si>
+    <t>developers/creating-modules/test-module.html</t>
+  </si>
+  <si>
+    <t>developers/creating-modules/use-module-creator.html</t>
+  </si>
+  <si>
+    <t>developers/developer-references.html</t>
+  </si>
+  <si>
+    <t>developers/extensions/dnn-manifest-schema.html</t>
+  </si>
+  <si>
+    <t>developers/extensions/index.html</t>
+  </si>
+  <si>
+    <t>developers/extensions/install-extension.html</t>
+  </si>
+  <si>
+    <t>developers/extensions/pack-extension.html</t>
+  </si>
+  <si>
+    <t>developers/glossary.html</t>
+  </si>
+  <si>
+    <t>developers/index.html</t>
+  </si>
+  <si>
+    <t>developers/providers.html</t>
+  </si>
+  <si>
+    <t>developers/requirements.html</t>
+  </si>
+  <si>
+    <t>developers/setup/index.html</t>
+  </si>
+  <si>
+    <t>developers/setup/run-installation-wizard.html</t>
+  </si>
+  <si>
+    <t>developers/setup/set-up-dnn-folder.html</t>
+  </si>
+  <si>
+    <t>developers/setup/set-up-dnn.html</t>
+  </si>
+  <si>
+    <t>developers/setup/set-up-iis.html</t>
+  </si>
+  <si>
+    <t>developers/setup/set-up-sql.html</t>
+  </si>
+  <si>
+    <t>Problems with infinite loop in web.config rules if the filenames are the same, case-insensitive.</t>
+  </si>
+  <si>
+    <t>administrators/dnn-platform-overview.html</t>
+  </si>
+  <si>
+    <t>administrators/whats-new-dnn8.html</t>
+  </si>
+  <si>
+    <t>designers/whats-new-dnn8.html</t>
+  </si>
+  <si>
+    <t>developers/whats-new-dnn8.html</t>
+  </si>
+  <si>
+    <t>designers/dnn-platform-overview.html</t>
+  </si>
+  <si>
+    <t>developers/dnn-platform-overview.html</t>
+  </si>
+  <si>
+    <t>administrators/security</t>
+  </si>
+  <si>
+    <t>administrators/security/jwt</t>
+  </si>
+  <si>
+    <t>administrators/security/roles</t>
+  </si>
+  <si>
+    <t>developers/security</t>
+  </si>
+  <si>
+    <t>developers/security/jwt</t>
+  </si>
+  <si>
+    <t>administrators/security/index.html</t>
+  </si>
+  <si>
+    <t>administrators/security/jwt/index.html</t>
+  </si>
+  <si>
+    <t>administrators/security/roles/index.html</t>
+  </si>
+  <si>
+    <t>developers/security/index.html</t>
+  </si>
+  <si>
+    <t>developers/security/jwt/index.html</t>
+  </si>
+  <si>
+    <t>/index.html</t>
+  </si>
+  <si>
+    <t>administrators/extensions/index.html</t>
+  </si>
+  <si>
     <t>administrators/</t>
   </si>
   <si>
@@ -780,6 +1044,15 @@
     <t>administrators/licensing/</t>
   </si>
   <si>
+    <t>administrators/security/</t>
+  </si>
+  <si>
+    <t>administrators/security/jwt/</t>
+  </si>
+  <si>
+    <t>administrators/security/roles/</t>
+  </si>
+  <si>
     <t>administrators/setup/</t>
   </si>
   <si>
@@ -807,289 +1080,16 @@
     <t>developers/extensions/</t>
   </si>
   <si>
+    <t>developers/security/</t>
+  </si>
+  <si>
+    <t>developers/security/jwt/</t>
+  </si>
+  <si>
     <t>developers/setup/</t>
   </si>
   <si>
-    <t>administrators/administrator-references.html</t>
-  </si>
-  <si>
-    <t>administrators/extensions/install-extension.html</t>
-  </si>
-  <si>
-    <t>administrators/glossary.html</t>
-  </si>
-  <si>
-    <t>administrators/index.html</t>
-  </si>
-  <si>
-    <t>administrators/licensing/activate-license-automatically.html</t>
-  </si>
-  <si>
-    <t>administrators/licensing/activate-license-manually.html</t>
-  </si>
-  <si>
-    <t>administrators/licensing/faq-licensing.html</t>
-  </si>
-  <si>
-    <t>administrators/licensing/index.html</t>
-  </si>
-  <si>
-    <t>administrators/licensing/licensing.html</t>
-  </si>
-  <si>
-    <t>administrators/licensing/troubleshooting-licensing.html</t>
-  </si>
-  <si>
-    <t>administrators/requirements.html</t>
-  </si>
-  <si>
-    <t>administrators/setup/index.html</t>
-  </si>
-  <si>
-    <t>administrators/setup/run-installation-wizard.html</t>
-  </si>
-  <si>
-    <t>administrators/setup/set-up-dnn-folder.html</t>
-  </si>
-  <si>
-    <t>administrators/setup/set-up-dnn.html</t>
-  </si>
-  <si>
-    <t>administrators/setup/set-up-iis.html</t>
-  </si>
-  <si>
-    <t>administrators/setup/set-up-sql.html</t>
-  </si>
-  <si>
-    <t>designers/about-themes.html</t>
-  </si>
-  <si>
-    <t>designers/creating-themes/create-container.html</t>
-  </si>
-  <si>
-    <t>designers/creating-themes/create-css.html</t>
-  </si>
-  <si>
-    <t>designers/creating-themes/create-doctype-xml.html</t>
-  </si>
-  <si>
-    <t>designers/creating-themes/create-layout-template.html</t>
-  </si>
-  <si>
-    <t>designers/creating-themes/create-theme.html</t>
-  </si>
-  <si>
-    <t>designers/creating-themes/index.html</t>
-  </si>
-  <si>
-    <t>designers/designer-references.html</t>
-  </si>
-  <si>
-    <t>designers/extensions/dnn-manifest-schema.html</t>
-  </si>
-  <si>
-    <t>designers/extensions/index.html</t>
-  </si>
-  <si>
-    <t>designers/extensions/install-extension.html</t>
-  </si>
-  <si>
-    <t>designers/extensions/pack-extension.html</t>
-  </si>
-  <si>
-    <t>designers/glossary.html</t>
-  </si>
-  <si>
-    <t>designers/index.html</t>
-  </si>
-  <si>
-    <t>designers/requirements.html</t>
-  </si>
-  <si>
-    <t>designers/setup/index.html</t>
-  </si>
-  <si>
-    <t>designers/setup/run-installation-wizard.html</t>
-  </si>
-  <si>
-    <t>designers/setup/set-up-dnn-folder.html</t>
-  </si>
-  <si>
-    <t>designers/setup/set-up-dnn.html</t>
-  </si>
-  <si>
-    <t>designers/setup/set-up-iis.html</t>
-  </si>
-  <si>
-    <t>designers/setup/set-up-sql.html</t>
-  </si>
-  <si>
-    <t>designers/theme-objects.html</t>
-  </si>
-  <si>
-    <t>developers/about-evs.html</t>
-  </si>
-  <si>
-    <t>developers/about-modules/index.html</t>
-  </si>
-  <si>
-    <t>developers/about-modules/module-architecture.html</t>
-  </si>
-  <si>
-    <t>developers/about-modules/module-development.html</t>
-  </si>
-  <si>
-    <t>developers/about-modules/module-features.html</t>
-  </si>
-  <si>
-    <t>developers/about-modules/mvc-module-development.html</t>
-  </si>
-  <si>
-    <t>developers/about-modules/spa-module-development.html</t>
-  </si>
-  <si>
-    <t>developers/about-modules/unsupported-mvc-features.html</t>
-  </si>
-  <si>
-    <t>developers/about-modules/web-forms-module-development.html</t>
-  </si>
-  <si>
-    <t>developers/creating-modules/create-module-using-templates.html</t>
-  </si>
-  <si>
-    <t>developers/creating-modules/create-module.html</t>
-  </si>
-  <si>
-    <t>developers/creating-modules/index.html</t>
-  </si>
-  <si>
-    <t>developers/creating-modules/start-vs-project-with-templates.html</t>
-  </si>
-  <si>
-    <t>developers/creating-modules/test-module.html</t>
-  </si>
-  <si>
-    <t>developers/creating-modules/use-module-creator.html</t>
-  </si>
-  <si>
-    <t>developers/developer-references.html</t>
-  </si>
-  <si>
-    <t>developers/extensions/dnn-manifest-schema.html</t>
-  </si>
-  <si>
-    <t>developers/extensions/index.html</t>
-  </si>
-  <si>
-    <t>developers/extensions/install-extension.html</t>
-  </si>
-  <si>
-    <t>developers/extensions/pack-extension.html</t>
-  </si>
-  <si>
-    <t>developers/glossary.html</t>
-  </si>
-  <si>
-    <t>developers/index.html</t>
-  </si>
-  <si>
-    <t>developers/providers.html</t>
-  </si>
-  <si>
-    <t>developers/requirements.html</t>
-  </si>
-  <si>
-    <t>developers/setup/index.html</t>
-  </si>
-  <si>
-    <t>developers/setup/run-installation-wizard.html</t>
-  </si>
-  <si>
-    <t>developers/setup/set-up-dnn-folder.html</t>
-  </si>
-  <si>
-    <t>developers/setup/set-up-dnn.html</t>
-  </si>
-  <si>
-    <t>developers/setup/set-up-iis.html</t>
-  </si>
-  <si>
-    <t>developers/setup/set-up-sql.html</t>
-  </si>
-  <si>
-    <t>Problems with infinite loop in web.config rules if the filenames are the same, case-insensitive.</t>
-  </si>
-  <si>
-    <t>administrators/dnn-platform-overview.html</t>
-  </si>
-  <si>
-    <t>administrators/whats-new-dnn8.html</t>
-  </si>
-  <si>
-    <t>designers/whats-new-dnn8.html</t>
-  </si>
-  <si>
-    <t>developers/whats-new-dnn8.html</t>
-  </si>
-  <si>
-    <t>designers/dnn-platform-overview.html</t>
-  </si>
-  <si>
-    <t>developers/dnn-platform-overview.html</t>
-  </si>
-  <si>
-    <t>administrators/security</t>
-  </si>
-  <si>
-    <t>administrators/security/</t>
-  </si>
-  <si>
-    <t>administrators/security/jwt</t>
-  </si>
-  <si>
-    <t>administrators/security/jwt/</t>
-  </si>
-  <si>
-    <t>administrators/security/roles</t>
-  </si>
-  <si>
-    <t>administrators/security/roles/</t>
-  </si>
-  <si>
-    <t>developers/security</t>
-  </si>
-  <si>
-    <t>developers/security/</t>
-  </si>
-  <si>
-    <t>developers/security/jwt</t>
-  </si>
-  <si>
-    <t>developers/security/jwt/</t>
-  </si>
-  <si>
-    <t>developers/security/roles</t>
-  </si>
-  <si>
-    <t>developers/security/roles/</t>
-  </si>
-  <si>
-    <t>administrators/security/index.html</t>
-  </si>
-  <si>
-    <t>administrators/security/jwt/index.html</t>
-  </si>
-  <si>
-    <t>administrators/security/roles/index.html</t>
-  </si>
-  <si>
-    <t>developers/security/index.html</t>
-  </si>
-  <si>
-    <t>developers/security/jwt/index.html</t>
-  </si>
-  <si>
-    <t>developers/security/roles/index.html</t>
+    <t>testonly</t>
   </si>
 </sst>
 </file>
@@ -1448,10 +1448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F133"/>
+  <dimension ref="A1:G118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D129" sqref="D129"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="D118" sqref="B2:D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1459,11 +1459,12 @@
     <col min="1" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="71.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="71.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="63.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="71.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2">
         <v>0</v>
       </c>
@@ -1473,11 +1474,11 @@
       <c r="D1" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <f>A1+1</f>
         <v>1</v>
@@ -1486,72 +1487,71 @@
         <f>CONCATENATE("Rule-",TEXT(A2,"000"))</f>
         <v>Rule-001</v>
       </c>
+      <c r="C2" t="s">
+        <v>231</v>
+      </c>
       <c r="D2" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>337</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <f t="shared" ref="A3:A66" si="0">A2+1</f>
+        <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="1" t="str">
-        <f t="shared" ref="B3:B66" si="1">CONCATENATE("Rule-",TEXT(A3,"000"))</f>
+        <f t="shared" ref="B3" si="0">CONCATENATE("Rule-",TEXT(A3,"000"))</f>
         <v>Rule-002</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <f t="shared" ref="A4:A8" si="1">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="str">
+        <f>CONCATENATE("Rule-",TEXT(A4,"000"))</f>
+        <v>Rule-003</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
-        <v>335</v>
-      </c>
-      <c r="E3" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="str">
-        <f t="shared" ref="B4:B16" si="2">CONCATENATE("Rule-",TEXT(A4,"000"))</f>
-        <v>Rule-003</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" t="s">
+        <v>322</v>
+      </c>
+      <c r="F4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="str">
+        <f t="shared" ref="B5:B17" si="2">CONCATENATE("Rule-",TEXT(A5,"000"))</f>
+        <v>Rule-004</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Rule-004</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="D5" t="s">
-        <v>274</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B6" s="1" t="str">
@@ -1559,15 +1559,19 @@
         <v>Rule-005</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B7" s="1" t="str">
@@ -1575,16 +1579,15 @@
         <v>Rule-006</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>266</v>
-      </c>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B8" s="1" t="str">
@@ -1592,28 +1595,32 @@
         <v>Rule-007</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A9:A67" si="3">A8+1</f>
         <v>8</v>
       </c>
       <c r="B9" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Rule-008</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="D9" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="B10" s="1" t="str">
@@ -1621,13 +1628,12 @@
         <v>Rule-009</v>
       </c>
       <c r="D10" t="s">
-        <v>269</v>
-      </c>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="B11" s="1" t="str">
@@ -1635,12 +1641,13 @@
         <v>Rule-010</v>
       </c>
       <c r="D11" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="B12" s="1" t="str">
@@ -1648,13 +1655,12 @@
         <v>Rule-011</v>
       </c>
       <c r="D12" t="s">
-        <v>271</v>
-      </c>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="B13" s="1" t="str">
@@ -1662,13 +1668,13 @@
         <v>Rule-012</v>
       </c>
       <c r="D13" t="s">
-        <v>272</v>
-      </c>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="B14" s="1" t="str">
@@ -1676,30 +1682,27 @@
         <v>Rule-013</v>
       </c>
       <c r="D14" t="s">
-        <v>273</v>
-      </c>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="B15" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Rule-014</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="D15" t="s">
-        <v>275</v>
-      </c>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="B16" s="1" t="str">
@@ -1707,1778 +1710,1544 @@
         <v>Rule-015</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>262</v>
+      </c>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Rule-016</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
+        <v>263</v>
+      </c>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="str">
+        <f t="shared" ref="B18:B67" si="4">CONCATENATE("Rule-",TEXT(A18,"000"))</f>
+        <v>Rule-017</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-018</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-019</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-020</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-021</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-022</v>
+      </c>
+      <c r="D23" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-023</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-024</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-025</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" t="s">
+        <v>271</v>
+      </c>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-026</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" t="s">
+        <v>272</v>
+      </c>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-027</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" t="s">
+        <v>273</v>
+      </c>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-028</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" t="s">
+        <v>274</v>
+      </c>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-029</v>
+      </c>
+      <c r="D30" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-030</v>
+      </c>
+      <c r="D31" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-031</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" t="s">
         <v>276</v>
       </c>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <f t="shared" si="0"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-032</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" t="s">
+        <v>277</v>
+      </c>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-033</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-034</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D35" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-035</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-036</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D37" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-037</v>
+      </c>
+      <c r="D38" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-038</v>
+      </c>
+      <c r="D39" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-039</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="B41" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-040</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-016</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <f t="shared" si="0"/>
+      <c r="D41" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="B42" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-041</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-017</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <f t="shared" si="0"/>
+      <c r="D42" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="B43" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-042</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="B44" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-043</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-018</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <f t="shared" si="0"/>
+      <c r="D44" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="B45" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-044</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-019</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B21" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-020</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="D45" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="B46" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-045</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D46" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="B47" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-046</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F47" s="1" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B22" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-021</v>
-      </c>
-      <c r="D22" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B23" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-022</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B24" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-023</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D24" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B25" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-024</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" t="s">
-        <v>284</v>
-      </c>
-      <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B26" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-025</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" t="s">
-        <v>285</v>
-      </c>
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <f t="shared" si="0"/>
+    <row r="48" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="B48" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-047</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-026</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D27" t="s">
-        <v>286</v>
-      </c>
-      <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="B28" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-027</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" t="s">
-        <v>287</v>
-      </c>
-      <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="B29" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-028</v>
-      </c>
-      <c r="D29" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="B30" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-029</v>
-      </c>
-      <c r="D30" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="B31" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-030</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D31" t="s">
-        <v>289</v>
-      </c>
-      <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="B32" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-031</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="D48" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="B49" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-048</v>
+      </c>
+      <c r="D49" t="s">
         <v>290</v>
       </c>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="B33" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-032</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D33" t="s">
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="B50" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-049</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D50" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="B34" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-033</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D34" t="s">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="B51" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-050</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D51" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <f t="shared" si="0"/>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <f t="shared" si="3"/>
+        <v>51</v>
+      </c>
+      <c r="B52" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-051</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D52" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <f t="shared" si="3"/>
+        <v>52</v>
+      </c>
+      <c r="B53" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-052</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D53" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <f t="shared" si="3"/>
+        <v>53</v>
+      </c>
+      <c r="B54" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-053</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D54" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <f t="shared" si="3"/>
+        <v>54</v>
+      </c>
+      <c r="B55" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-054</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D55" t="s">
+        <v>296</v>
+      </c>
+      <c r="G55" s="1"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <f t="shared" si="3"/>
+        <v>55</v>
+      </c>
+      <c r="B56" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-055</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D56" t="s">
+        <v>297</v>
+      </c>
+      <c r="G56" s="1"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <f t="shared" si="3"/>
+        <v>56</v>
+      </c>
+      <c r="B57" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-056</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D57" t="s">
+        <v>298</v>
+      </c>
+      <c r="G57" s="1"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <f t="shared" si="3"/>
+        <v>57</v>
+      </c>
+      <c r="B58" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-057</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D58" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <f t="shared" si="3"/>
+        <v>58</v>
+      </c>
+      <c r="B59" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-058</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D59" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <f t="shared" si="3"/>
+        <v>59</v>
+      </c>
+      <c r="B60" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-059</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D60" t="s">
+        <v>301</v>
+      </c>
+      <c r="G60" s="1"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="B61" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-060</v>
+      </c>
+      <c r="D61" t="s">
+        <v>302</v>
+      </c>
+      <c r="G61" s="1"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <f t="shared" si="3"/>
+        <v>61</v>
+      </c>
+      <c r="B62" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-061</v>
+      </c>
+      <c r="D62" t="s">
+        <v>303</v>
+      </c>
+      <c r="G62" s="1"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <f t="shared" si="3"/>
+        <v>62</v>
+      </c>
+      <c r="B63" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-062</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D63" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <f t="shared" si="3"/>
+        <v>63</v>
+      </c>
+      <c r="B64" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-063</v>
+      </c>
+      <c r="D64" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <f t="shared" si="3"/>
+        <v>64</v>
+      </c>
+      <c r="B65" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-064</v>
+      </c>
+      <c r="D65" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <f t="shared" si="3"/>
+        <v>65</v>
+      </c>
+      <c r="B66" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-065</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D66" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <f t="shared" si="3"/>
+        <v>66</v>
+      </c>
+      <c r="B67" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Rule-066</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D67" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <f t="shared" ref="A68:A79" si="5">A67+1</f>
+        <v>67</v>
+      </c>
+      <c r="B68" s="1" t="str">
+        <f t="shared" ref="B68:B83" si="6">CONCATENATE("Rule-",TEXT(A68,"000"))</f>
+        <v>Rule-067</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D68" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <f t="shared" si="5"/>
+        <v>68</v>
+      </c>
+      <c r="B69" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Rule-068</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D69" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <f t="shared" si="5"/>
+        <v>69</v>
+      </c>
+      <c r="B70" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Rule-069</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D70" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <f t="shared" si="5"/>
+        <v>70</v>
+      </c>
+      <c r="B71" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Rule-070</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D71" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <f t="shared" si="5"/>
+        <v>71</v>
+      </c>
+      <c r="B72" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Rule-071</v>
+      </c>
+      <c r="D72" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <f t="shared" si="5"/>
+        <v>72</v>
+      </c>
+      <c r="B73" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Rule-072</v>
+      </c>
+      <c r="D73" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <f t="shared" si="5"/>
+        <v>73</v>
+      </c>
+      <c r="B74" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Rule-073</v>
+      </c>
+      <c r="D74" t="s">
+        <v>313</v>
+      </c>
+      <c r="G74" s="1"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <f t="shared" si="5"/>
+        <v>74</v>
+      </c>
+      <c r="B75" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Rule-074</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D75" t="s">
+        <v>314</v>
+      </c>
+      <c r="G75" s="1"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <f t="shared" si="5"/>
+        <v>75</v>
+      </c>
+      <c r="B76" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Rule-075</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D76" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <f t="shared" si="5"/>
+        <v>76</v>
+      </c>
+      <c r="B77" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Rule-076</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D77" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <f t="shared" si="5"/>
+        <v>77</v>
+      </c>
+      <c r="B78" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Rule-077</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D78" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <f t="shared" si="5"/>
+        <v>78</v>
+      </c>
+      <c r="B79" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Rule-078</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D79" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <f t="shared" ref="A80:A82" si="7">A79+1</f>
+        <v>79</v>
+      </c>
+      <c r="B80" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Rule-079</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D80" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <f t="shared" si="7"/>
+        <v>80</v>
+      </c>
+      <c r="B81" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Rule-080</v>
+      </c>
+      <c r="C81" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-034</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D35" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="B36" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-035</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D36" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="B37" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-036</v>
-      </c>
-      <c r="D37" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="B38" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-037</v>
-      </c>
-      <c r="D38" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="B39" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-038</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D39" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-      <c r="B40" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-039</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D40" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="B41" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-040</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D41" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="B42" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-041</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D42" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="B43" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-042</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D43" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="B44" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-043</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D44" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="B45" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-044</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D45" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="B46" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-045</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E46" s="1" t="s">
+      <c r="D81" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F81" s="1" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="B47" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-046</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="B48" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-047</v>
-      </c>
-      <c r="D48" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="B49" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-048</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D49" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="B50" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-049</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D50" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="B51" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-050</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D51" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
-      <c r="B52" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-051</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D52" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
-        <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
-      <c r="B53" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-052</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D53" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
-        <f t="shared" si="0"/>
-        <v>53</v>
-      </c>
-      <c r="B54" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-053</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D54" t="s">
-        <v>309</v>
-      </c>
-      <c r="F54" s="1"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-      <c r="B55" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-054</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D55" t="s">
-        <v>310</v>
-      </c>
-      <c r="F55" s="1"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
-        <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-      <c r="B56" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-055</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D56" t="s">
-        <v>311</v>
-      </c>
-      <c r="F56" s="1"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
-        <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
-      <c r="B57" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-056</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D57" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
-        <f t="shared" si="0"/>
-        <v>57</v>
-      </c>
-      <c r="B58" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-057</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D58" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
-        <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
-      <c r="B59" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-058</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D59" t="s">
-        <v>314</v>
-      </c>
-      <c r="F59" s="1"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="1">
-        <f t="shared" si="0"/>
-        <v>59</v>
-      </c>
-      <c r="B60" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-059</v>
-      </c>
-      <c r="D60" t="s">
-        <v>315</v>
-      </c>
-      <c r="F60" s="1"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="B61" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-060</v>
-      </c>
-      <c r="D61" t="s">
-        <v>316</v>
-      </c>
-      <c r="F61" s="1"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
-        <f t="shared" si="0"/>
-        <v>61</v>
-      </c>
-      <c r="B62" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-061</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D62" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
-        <f t="shared" si="0"/>
-        <v>62</v>
-      </c>
-      <c r="B63" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-062</v>
-      </c>
-      <c r="D63" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="1">
-        <f t="shared" si="0"/>
-        <v>63</v>
-      </c>
-      <c r="B64" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-063</v>
-      </c>
-      <c r="D64" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="1">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="B65" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-064</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D65" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="1">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
-      <c r="B66" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Rule-065</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D66" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="1">
-        <f t="shared" ref="A67:A78" si="3">A66+1</f>
-        <v>66</v>
-      </c>
-      <c r="B67" s="1" t="str">
-        <f t="shared" ref="B67:B87" si="4">CONCATENATE("Rule-",TEXT(A67,"000"))</f>
-        <v>Rule-066</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D67" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
-        <f t="shared" si="3"/>
-        <v>67</v>
-      </c>
-      <c r="B68" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-067</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D68" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="1">
-        <f t="shared" si="3"/>
-        <v>68</v>
-      </c>
-      <c r="B69" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-068</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D69" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
-        <f t="shared" si="3"/>
-        <v>69</v>
-      </c>
-      <c r="B70" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-069</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D70" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
-        <f t="shared" si="3"/>
-        <v>70</v>
-      </c>
-      <c r="B71" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-070</v>
-      </c>
-      <c r="D71" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
-        <f t="shared" si="3"/>
-        <v>71</v>
-      </c>
-      <c r="B72" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-071</v>
-      </c>
-      <c r="D72" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
-        <f t="shared" si="3"/>
-        <v>72</v>
-      </c>
-      <c r="B73" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-072</v>
-      </c>
-      <c r="D73" t="s">
-        <v>326</v>
-      </c>
-      <c r="F73" s="1"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
-        <f t="shared" si="3"/>
-        <v>73</v>
-      </c>
-      <c r="B74" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-073</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D74" t="s">
-        <v>327</v>
-      </c>
-      <c r="F74" s="1"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="1">
-        <f t="shared" si="3"/>
-        <v>74</v>
-      </c>
-      <c r="B75" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-074</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D75" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
-        <f t="shared" si="3"/>
-        <v>75</v>
-      </c>
-      <c r="B76" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-075</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D76" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
-        <f t="shared" si="3"/>
-        <v>76</v>
-      </c>
-      <c r="B77" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-076</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D77" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="1">
-        <f t="shared" si="3"/>
-        <v>77</v>
-      </c>
-      <c r="B78" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-077</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D78" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
-        <f t="shared" ref="A79:A81" si="5">A78+1</f>
-        <v>78</v>
-      </c>
-      <c r="B79" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-078</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D79" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="1">
-        <f t="shared" si="5"/>
-        <v>79</v>
-      </c>
-      <c r="B80" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-079</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="1">
-        <f t="shared" si="5"/>
-        <v>80</v>
-      </c>
-      <c r="B81" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-080</v>
-      </c>
-      <c r="D81" t="s">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <f t="shared" si="7"/>
+        <v>81</v>
+      </c>
+      <c r="B82" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Rule-081</v>
+      </c>
+      <c r="D82" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="1">
-        <f t="shared" ref="A82:A119" si="6">A81+1</f>
-        <v>81</v>
-      </c>
-      <c r="B82" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-081</v>
-      </c>
-      <c r="C82" t="s">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <f t="shared" ref="A83:A100" si="8">A82+1</f>
+        <v>82</v>
+      </c>
+      <c r="B83" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Rule-082</v>
+      </c>
+      <c r="C83" t="s">
         <v>238</v>
       </c>
-      <c r="D82" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="E82" s="1" t="s">
+      <c r="D83" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="F83" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="1">
-        <f t="shared" si="6"/>
-        <v>82</v>
-      </c>
-      <c r="B83" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-082</v>
-      </c>
-      <c r="C83" t="s">
-        <v>251</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>83</v>
       </c>
       <c r="B84" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="B84:B99" si="9">CONCATENATE("Rule-",TEXT(A84,"000"))</f>
         <v>Rule-083</v>
       </c>
       <c r="C84" t="s">
         <v>241</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="E84" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="F84" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>84</v>
       </c>
       <c r="B85" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>Rule-084</v>
       </c>
       <c r="C85" t="s">
-        <v>252</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="E85" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D85" t="s">
+        <v>258</v>
+      </c>
+      <c r="F85" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>85</v>
       </c>
       <c r="B86" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>Rule-085</v>
       </c>
-      <c r="C86" t="s">
-        <v>242</v>
-      </c>
-      <c r="D86" t="s">
-        <v>271</v>
-      </c>
-      <c r="E86" s="1" t="s">
+      <c r="C86" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="F86" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>86</v>
       </c>
       <c r="B87" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>Rule-086</v>
       </c>
-      <c r="C87" t="s">
-        <v>253</v>
+      <c r="C87" s="1" t="s">
+        <v>328</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="E87" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="F87" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>87</v>
       </c>
       <c r="B88" s="1" t="str">
-        <f t="shared" ref="B88:B119" si="7">CONCATENATE("Rule-",TEXT(A88,"000"))</f>
+        <f t="shared" si="9"/>
         <v>Rule-087</v>
       </c>
       <c r="C88" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <f t="shared" si="8"/>
+        <v>88</v>
+      </c>
+      <c r="B89" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>Rule-088</v>
+      </c>
+      <c r="C89" t="s">
+        <v>243</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <f t="shared" si="8"/>
+        <v>89</v>
+      </c>
+      <c r="B90" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>Rule-089</v>
+      </c>
+      <c r="C90" t="s">
+        <v>239</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <f t="shared" si="8"/>
+        <v>90</v>
+      </c>
+      <c r="B91" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>Rule-090</v>
+      </c>
+      <c r="C91" t="s">
+        <v>244</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <f t="shared" si="8"/>
+        <v>91</v>
+      </c>
+      <c r="B92" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>Rule-091</v>
+      </c>
+      <c r="C92" t="s">
+        <v>245</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <f t="shared" si="8"/>
+        <v>92</v>
+      </c>
+      <c r="B93" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>Rule-092</v>
+      </c>
+      <c r="C93" t="s">
+        <v>246</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <f t="shared" si="8"/>
+        <v>93</v>
+      </c>
+      <c r="B94" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>Rule-093</v>
+      </c>
+      <c r="C94" t="s">
+        <v>240</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <f t="shared" si="8"/>
+        <v>94</v>
+      </c>
+      <c r="B95" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>Rule-094</v>
+      </c>
+      <c r="C95" t="s">
+        <v>247</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <f t="shared" si="8"/>
+        <v>95</v>
+      </c>
+      <c r="B96" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>Rule-095</v>
+      </c>
+      <c r="C96" t="s">
+        <v>248</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <f t="shared" si="8"/>
+        <v>96</v>
+      </c>
+      <c r="B97" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>Rule-096</v>
+      </c>
+      <c r="C97" t="s">
+        <v>249</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <f t="shared" si="8"/>
+        <v>97</v>
+      </c>
+      <c r="B98" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>Rule-097</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <f t="shared" si="8"/>
+        <v>98</v>
+      </c>
+      <c r="B99" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>Rule-098</v>
+      </c>
+      <c r="C99" t="s">
+        <v>331</v>
+      </c>
+      <c r="D99" t="s">
+        <v>336</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <f t="shared" si="8"/>
+        <v>99</v>
+      </c>
+      <c r="B100" s="1" t="str">
+        <f t="shared" ref="B100" si="10">CONCATENATE("Rule-",TEXT(A100,"000"))</f>
+        <v>Rule-099</v>
+      </c>
+      <c r="C100" t="s">
+        <v>250</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B101" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B102" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C102" t="s">
         <v>340</v>
       </c>
-      <c r="D88" s="1" t="s">
+    </row>
+    <row r="103" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B103" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B104" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B105" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B106" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B107" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B108" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B109" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B110" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B111" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B112" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="113" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B113" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C113" t="s">
+        <v>351</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="114" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B114" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C114" t="s">
         <v>352</v>
       </c>
-      <c r="E88" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="1">
-        <f t="shared" si="6"/>
-        <v>88</v>
-      </c>
-      <c r="B89" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Rule-088</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="E89" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="1">
-        <f t="shared" si="6"/>
-        <v>89</v>
-      </c>
-      <c r="B90" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Rule-089</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="D90" s="1" t="s">
+      <c r="F114" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="115" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B115" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C115" t="s">
         <v>353</v>
       </c>
-      <c r="E90" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="1">
-        <f t="shared" si="6"/>
-        <v>90</v>
-      </c>
-      <c r="B91" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Rule-090</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="1">
-        <f t="shared" si="6"/>
-        <v>91</v>
-      </c>
-      <c r="B92" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Rule-091</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="D92" s="1" t="s">
+    </row>
+    <row r="116" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B116" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C116" t="s">
         <v>354</v>
       </c>
-      <c r="E92" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="1">
-        <f t="shared" si="6"/>
-        <v>92</v>
-      </c>
-      <c r="B93" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Rule-092</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="1">
-        <f t="shared" si="6"/>
-        <v>93</v>
-      </c>
-      <c r="B94" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Rule-093</v>
-      </c>
-      <c r="C94" t="s">
-        <v>243</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="1">
-        <f t="shared" si="6"/>
-        <v>94</v>
-      </c>
-      <c r="B95" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Rule-094</v>
-      </c>
-      <c r="C95" t="s">
-        <v>254</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="1">
-        <f t="shared" si="6"/>
-        <v>95</v>
-      </c>
-      <c r="B96" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Rule-095</v>
-      </c>
-      <c r="C96" t="s">
-        <v>239</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="1">
-        <f t="shared" si="6"/>
-        <v>96</v>
-      </c>
-      <c r="B97" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Rule-096</v>
-      </c>
-      <c r="C97" t="s">
-        <v>255</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="1">
-        <f t="shared" si="6"/>
-        <v>97</v>
-      </c>
-      <c r="B98" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Rule-097</v>
-      </c>
-      <c r="C98" t="s">
-        <v>244</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="1">
-        <f t="shared" si="6"/>
-        <v>98</v>
-      </c>
-      <c r="B99" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Rule-098</v>
-      </c>
-      <c r="C99" t="s">
-        <v>256</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="1">
-        <f t="shared" si="6"/>
-        <v>99</v>
-      </c>
-      <c r="B100" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Rule-099</v>
-      </c>
-      <c r="C100" t="s">
-        <v>245</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="1">
-        <f t="shared" si="6"/>
-        <v>100</v>
-      </c>
-      <c r="B101" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Rule-100</v>
-      </c>
-      <c r="C101" t="s">
-        <v>257</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="1">
-        <f t="shared" si="6"/>
-        <v>101</v>
-      </c>
-      <c r="B102" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Rule-101</v>
-      </c>
-      <c r="C102" t="s">
-        <v>246</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="1">
-        <f t="shared" si="6"/>
-        <v>102</v>
-      </c>
-      <c r="B103" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Rule-102</v>
-      </c>
-      <c r="C103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="1">
-        <f t="shared" si="6"/>
-        <v>103</v>
-      </c>
-      <c r="B104" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Rule-103</v>
-      </c>
-      <c r="C104" t="s">
-        <v>240</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" s="1">
-        <f t="shared" si="6"/>
-        <v>104</v>
-      </c>
-      <c r="B105" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Rule-104</v>
-      </c>
-      <c r="C105" t="s">
-        <v>259</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" s="1">
-        <f t="shared" si="6"/>
-        <v>105</v>
-      </c>
-      <c r="B106" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Rule-105</v>
-      </c>
-      <c r="C106" t="s">
-        <v>247</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="E106" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" s="1">
-        <f t="shared" si="6"/>
-        <v>106</v>
-      </c>
-      <c r="B107" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Rule-106</v>
-      </c>
-      <c r="C107" t="s">
-        <v>260</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" s="1">
-        <f t="shared" si="6"/>
-        <v>107</v>
-      </c>
-      <c r="B108" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Rule-107</v>
-      </c>
-      <c r="C108" t="s">
-        <v>248</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="E108" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" s="1">
-        <f t="shared" si="6"/>
-        <v>108</v>
-      </c>
-      <c r="B109" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Rule-108</v>
-      </c>
-      <c r="C109" t="s">
-        <v>261</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" s="1">
-        <f t="shared" si="6"/>
-        <v>109</v>
-      </c>
-      <c r="B110" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Rule-109</v>
-      </c>
-      <c r="C110" t="s">
-        <v>249</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" s="1">
-        <f t="shared" si="6"/>
-        <v>110</v>
-      </c>
-      <c r="B111" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Rule-110</v>
-      </c>
-      <c r="C111" t="s">
-        <v>262</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="E111" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="1">
-        <f t="shared" si="6"/>
-        <v>111</v>
-      </c>
-      <c r="B112" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Rule-111</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="D112" s="1" t="s">
+    </row>
+    <row r="117" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B117" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C117" t="s">
         <v>355</v>
       </c>
-      <c r="E112" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="1">
-        <f t="shared" si="6"/>
-        <v>112</v>
-      </c>
-      <c r="B113" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Rule-112</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="E113" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" s="1">
-        <f t="shared" si="6"/>
-        <v>113</v>
-      </c>
-      <c r="B114" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Rule-113</v>
-      </c>
-      <c r="C114" t="s">
-        <v>348</v>
-      </c>
-      <c r="D114" t="s">
+    </row>
+    <row r="118" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B118" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C118" t="s">
         <v>356</v>
-      </c>
-      <c r="E114" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" s="1">
-        <f t="shared" si="6"/>
-        <v>114</v>
-      </c>
-      <c r="B115" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Rule-114</v>
-      </c>
-      <c r="C115" t="s">
-        <v>349</v>
-      </c>
-      <c r="D115" t="s">
-        <v>356</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" s="1">
-        <f t="shared" si="6"/>
-        <v>115</v>
-      </c>
-      <c r="B116" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Rule-115</v>
-      </c>
-      <c r="C116" t="s">
-        <v>350</v>
-      </c>
-      <c r="D116" t="s">
-        <v>357</v>
-      </c>
-      <c r="E116" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="1">
-        <f t="shared" si="6"/>
-        <v>116</v>
-      </c>
-      <c r="B117" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Rule-116</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="E117" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118" s="1">
-        <f t="shared" si="6"/>
-        <v>117</v>
-      </c>
-      <c r="B118" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Rule-117</v>
-      </c>
-      <c r="C118" t="s">
-        <v>250</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="E118" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" s="1">
-        <f t="shared" si="6"/>
-        <v>118</v>
-      </c>
-      <c r="B119" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Rule-118</v>
-      </c>
-      <c r="C119" t="s">
-        <v>263</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="122" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="123" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="124" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="125" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="126" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="127" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="128" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="129" spans="5:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="130" spans="5:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="131" spans="5:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="132" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E132" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="133" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E133" s="1" t="s">
-        <v>237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Included Modules: Added new topics. administrators/licensing/*.dita: Added prodinfo tags. DNN license: Fixed trademark tags. security.ditamap; Removed topicset tags. designers/theme-objects.dita: Added navtitle. web.config, urlmap: Updated index.html rules for new folders. bld.bat, expectedfiles.txt: Updated build and tests.
</commit_message>
<xml_diff>
--- a/_build/urlmap/DC-URLmapping.xlsx
+++ b/_build/urlmap/DC-URLmapping.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="365">
   <si>
     <t>DNN8-Requirements.html</t>
   </si>
@@ -726,12 +726,6 @@
     <t>external</t>
   </si>
   <si>
-    <t>Causes an infinite loop: index.html</t>
-  </si>
-  <si>
-    <t>Causes an infinite loop: /</t>
-  </si>
-  <si>
     <t>administrators</t>
   </si>
   <si>
@@ -1090,6 +1084,33 @@
   </si>
   <si>
     <t>testonly</t>
+  </si>
+  <si>
+    <t>administrators/included-modules</t>
+  </si>
+  <si>
+    <t>designers/included-modules</t>
+  </si>
+  <si>
+    <t>developers/included-modules</t>
+  </si>
+  <si>
+    <t>administrators/included-modules/</t>
+  </si>
+  <si>
+    <t>designers/included-modules/</t>
+  </si>
+  <si>
+    <t>developers/included-modules/</t>
+  </si>
+  <si>
+    <t>administrators/included-modules/index.html</t>
+  </si>
+  <si>
+    <t>designers/included-modules/index.html</t>
+  </si>
+  <si>
+    <t>developers/included-modules/index.html</t>
   </si>
 </sst>
 </file>
@@ -1448,10 +1469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G118"/>
+  <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="D118" sqref="B2:D118"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B124" sqref="B2:D124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1491,7 +1512,7 @@
         <v>231</v>
       </c>
       <c r="D2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>224</v>
@@ -1507,7 +1528,7 @@
         <v>Rule-002</v>
       </c>
       <c r="D3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1523,10 +1544,10 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F4" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1542,10 +1563,10 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -1562,10 +1583,10 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G6" s="1"/>
     </row>
@@ -1582,7 +1603,7 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1598,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G8" s="1"/>
     </row>
@@ -1615,7 +1636,7 @@
         <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1628,7 +1649,7 @@
         <v>Rule-009</v>
       </c>
       <c r="D10" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1641,7 +1662,7 @@
         <v>Rule-010</v>
       </c>
       <c r="D11" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G11" s="1"/>
     </row>
@@ -1655,7 +1676,7 @@
         <v>Rule-011</v>
       </c>
       <c r="D12" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1668,7 +1689,7 @@
         <v>Rule-012</v>
       </c>
       <c r="D13" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="G13" s="1"/>
     </row>
@@ -1682,7 +1703,7 @@
         <v>Rule-013</v>
       </c>
       <c r="D14" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G14" s="1"/>
     </row>
@@ -1696,7 +1717,7 @@
         <v>Rule-014</v>
       </c>
       <c r="D15" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G15" s="1"/>
     </row>
@@ -1713,7 +1734,7 @@
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="G16" s="1"/>
     </row>
@@ -1730,7 +1751,7 @@
         <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G17" s="1"/>
     </row>
@@ -1747,7 +1768,7 @@
         <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1763,7 +1784,7 @@
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1779,7 +1800,7 @@
         <v>8</v>
       </c>
       <c r="D20" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1795,7 +1816,7 @@
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1827,7 +1848,7 @@
         <v>Rule-022</v>
       </c>
       <c r="D23" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1843,7 +1864,7 @@
         <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1859,7 +1880,7 @@
         <v>21</v>
       </c>
       <c r="D25" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1875,7 +1896,7 @@
         <v>23</v>
       </c>
       <c r="D26" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G26" s="1"/>
     </row>
@@ -1892,7 +1913,7 @@
         <v>24</v>
       </c>
       <c r="D27" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G27" s="1"/>
     </row>
@@ -1909,7 +1930,7 @@
         <v>25</v>
       </c>
       <c r="D28" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G28" s="1"/>
     </row>
@@ -1926,7 +1947,7 @@
         <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G29" s="1"/>
     </row>
@@ -1940,7 +1961,7 @@
         <v>Rule-029</v>
       </c>
       <c r="D30" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1953,7 +1974,7 @@
         <v>Rule-030</v>
       </c>
       <c r="D31" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1969,7 +1990,7 @@
         <v>29</v>
       </c>
       <c r="D32" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G32" s="1"/>
     </row>
@@ -1986,7 +2007,7 @@
         <v>30</v>
       </c>
       <c r="D33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="G33" s="1"/>
     </row>
@@ -2003,7 +2024,7 @@
         <v>14</v>
       </c>
       <c r="D34" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -2019,7 +2040,7 @@
         <v>28</v>
       </c>
       <c r="D35" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -2035,7 +2056,7 @@
         <v>20</v>
       </c>
       <c r="D36" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -2051,7 +2072,7 @@
         <v>33</v>
       </c>
       <c r="D37" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -2064,7 +2085,7 @@
         <v>Rule-037</v>
       </c>
       <c r="D38" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -2077,7 +2098,7 @@
         <v>Rule-038</v>
       </c>
       <c r="D39" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -2093,7 +2114,7 @@
         <v>13</v>
       </c>
       <c r="D40" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -2109,7 +2130,7 @@
         <v>16</v>
       </c>
       <c r="D41" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -2125,7 +2146,7 @@
         <v>17</v>
       </c>
       <c r="D42" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -2141,7 +2162,7 @@
         <v>15</v>
       </c>
       <c r="D43" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -2157,7 +2178,7 @@
         <v>18</v>
       </c>
       <c r="D44" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -2173,7 +2194,7 @@
         <v>19</v>
       </c>
       <c r="D45" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -2189,7 +2210,7 @@
         <v>32</v>
       </c>
       <c r="D46" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="47" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2224,7 +2245,7 @@
         <v>26</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>234</v>
@@ -2240,7 +2261,7 @@
         <v>Rule-048</v>
       </c>
       <c r="D49" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -2256,7 +2277,7 @@
         <v>35</v>
       </c>
       <c r="D50" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -2272,7 +2293,7 @@
         <v>38</v>
       </c>
       <c r="D51" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -2288,7 +2309,7 @@
         <v>36</v>
       </c>
       <c r="D52" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -2304,7 +2325,7 @@
         <v>39</v>
       </c>
       <c r="D53" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -2320,7 +2341,7 @@
         <v>37</v>
       </c>
       <c r="D54" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -2336,7 +2357,7 @@
         <v>40</v>
       </c>
       <c r="D55" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G55" s="1"/>
     </row>
@@ -2353,7 +2374,7 @@
         <v>41</v>
       </c>
       <c r="D56" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="G56" s="1"/>
     </row>
@@ -2370,7 +2391,7 @@
         <v>42</v>
       </c>
       <c r="D57" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G57" s="1"/>
     </row>
@@ -2387,7 +2408,7 @@
         <v>51</v>
       </c>
       <c r="D58" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -2403,7 +2424,7 @@
         <v>52</v>
       </c>
       <c r="D59" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -2419,7 +2440,7 @@
         <v>54</v>
       </c>
       <c r="D60" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G60" s="1"/>
     </row>
@@ -2433,7 +2454,7 @@
         <v>Rule-060</v>
       </c>
       <c r="D61" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="G61" s="1"/>
     </row>
@@ -2447,7 +2468,7 @@
         <v>Rule-061</v>
       </c>
       <c r="D62" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="G62" s="1"/>
     </row>
@@ -2464,7 +2485,7 @@
         <v>53</v>
       </c>
       <c r="D63" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -2477,7 +2498,7 @@
         <v>Rule-063</v>
       </c>
       <c r="D64" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -2490,7 +2511,7 @@
         <v>Rule-064</v>
       </c>
       <c r="D65" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -2506,7 +2527,7 @@
         <v>56</v>
       </c>
       <c r="D66" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -2522,7 +2543,7 @@
         <v>57</v>
       </c>
       <c r="D67" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -2531,14 +2552,14 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="str">
-        <f t="shared" ref="B68:B83" si="6">CONCATENATE("Rule-",TEXT(A68,"000"))</f>
+        <f t="shared" ref="B68:B81" si="6">CONCATENATE("Rule-",TEXT(A68,"000"))</f>
         <v>Rule-067</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D68" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -2554,7 +2575,7 @@
         <v>55</v>
       </c>
       <c r="D69" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -2570,7 +2591,7 @@
         <v>50</v>
       </c>
       <c r="D70" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -2586,7 +2607,7 @@
         <v>58</v>
       </c>
       <c r="D71" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -2599,7 +2620,7 @@
         <v>Rule-071</v>
       </c>
       <c r="D72" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -2612,7 +2633,7 @@
         <v>Rule-072</v>
       </c>
       <c r="D73" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -2625,7 +2646,7 @@
         <v>Rule-073</v>
       </c>
       <c r="D74" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G74" s="1"/>
     </row>
@@ -2642,7 +2663,7 @@
         <v>43</v>
       </c>
       <c r="D75" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="G75" s="1"/>
     </row>
@@ -2659,7 +2680,7 @@
         <v>46</v>
       </c>
       <c r="D76" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -2675,7 +2696,7 @@
         <v>47</v>
       </c>
       <c r="D77" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -2691,7 +2712,7 @@
         <v>45</v>
       </c>
       <c r="D78" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -2707,12 +2728,12 @@
         <v>48</v>
       </c>
       <c r="D79" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <f t="shared" ref="A80:A82" si="7">A79+1</f>
+        <f t="shared" ref="A80:A103" si="7">A79+1</f>
         <v>79</v>
       </c>
       <c r="B80" s="1" t="str">
@@ -2723,7 +2744,7 @@
         <v>49</v>
       </c>
       <c r="D80" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -2751,7 +2772,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="B82:B103" si="8">CONCATENATE("Rule-",TEXT(A82,"000"))</f>
         <v>Rule-081</v>
       </c>
       <c r="D82" t="s">
@@ -2760,18 +2781,18 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <f t="shared" ref="A83:A100" si="8">A82+1</f>
+        <f t="shared" si="7"/>
         <v>82</v>
       </c>
       <c r="B83" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>Rule-082</v>
       </c>
       <c r="C83" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>224</v>
@@ -2779,18 +2800,18 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
+        <f t="shared" si="7"/>
+        <v>83</v>
+      </c>
+      <c r="B84" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>83</v>
-      </c>
-      <c r="B84" s="1" t="str">
-        <f t="shared" ref="B84:B99" si="9">CONCATENATE("Rule-",TEXT(A84,"000"))</f>
         <v>Rule-083</v>
       </c>
       <c r="C84" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>224</v>
@@ -2798,18 +2819,18 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
+        <f t="shared" si="7"/>
+        <v>84</v>
+      </c>
+      <c r="B85" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>84</v>
-      </c>
-      <c r="B85" s="1" t="str">
-        <f t="shared" si="9"/>
         <v>Rule-084</v>
       </c>
-      <c r="C85" t="s">
-        <v>242</v>
-      </c>
-      <c r="D85" t="s">
-        <v>258</v>
+      <c r="C85" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>362</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>224</v>
@@ -2817,37 +2838,37 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
+        <f t="shared" si="7"/>
+        <v>85</v>
+      </c>
+      <c r="B86" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>85</v>
-      </c>
-      <c r="B86" s="1" t="str">
-        <f t="shared" si="9"/>
         <v>Rule-085</v>
       </c>
-      <c r="C86" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>332</v>
+      <c r="C86" t="s">
+        <v>240</v>
+      </c>
+      <c r="D86" t="s">
+        <v>256</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="87" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
+        <f t="shared" si="7"/>
+        <v>86</v>
+      </c>
+      <c r="B87" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>86</v>
-      </c>
-      <c r="B87" s="1" t="str">
-        <f t="shared" si="9"/>
         <v>Rule-086</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>224</v>
@@ -2855,37 +2876,37 @@
     </row>
     <row r="88" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
+        <f t="shared" si="7"/>
+        <v>87</v>
+      </c>
+      <c r="B88" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>87</v>
-      </c>
-      <c r="B88" s="1" t="str">
-        <f t="shared" si="9"/>
         <v>Rule-087</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
+        <f t="shared" si="7"/>
+        <v>88</v>
+      </c>
+      <c r="B89" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>88</v>
-      </c>
-      <c r="B89" s="1" t="str">
-        <f t="shared" si="9"/>
         <v>Rule-088</v>
       </c>
-      <c r="C89" t="s">
-        <v>243</v>
+      <c r="C89" s="1" t="s">
+        <v>327</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>262</v>
+        <v>332</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>224</v>
@@ -2893,18 +2914,18 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
+        <f t="shared" si="7"/>
+        <v>89</v>
+      </c>
+      <c r="B90" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>89</v>
-      </c>
-      <c r="B90" s="1" t="str">
-        <f t="shared" si="9"/>
         <v>Rule-089</v>
       </c>
       <c r="C90" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>281</v>
+        <v>260</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>224</v>
@@ -2912,18 +2933,18 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
+        <f t="shared" si="7"/>
+        <v>90</v>
+      </c>
+      <c r="B91" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>90</v>
-      </c>
-      <c r="B91" s="1" t="str">
-        <f t="shared" si="9"/>
         <v>Rule-090</v>
       </c>
       <c r="C91" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>224</v>
@@ -2931,18 +2952,18 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
+        <f t="shared" si="7"/>
+        <v>91</v>
+      </c>
+      <c r="B92" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>91</v>
-      </c>
-      <c r="B92" s="1" t="str">
-        <f t="shared" si="9"/>
         <v>Rule-091</v>
       </c>
       <c r="C92" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>224</v>
@@ -2950,18 +2971,18 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
+        <f t="shared" si="7"/>
+        <v>92</v>
+      </c>
+      <c r="B93" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>92</v>
-      </c>
-      <c r="B93" s="1" t="str">
-        <f t="shared" si="9"/>
         <v>Rule-092</v>
       </c>
       <c r="C93" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>224</v>
@@ -2969,18 +2990,18 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
+        <f t="shared" si="7"/>
+        <v>93</v>
+      </c>
+      <c r="B94" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>93</v>
-      </c>
-      <c r="B94" s="1" t="str">
-        <f t="shared" si="9"/>
         <v>Rule-093</v>
       </c>
-      <c r="C94" t="s">
-        <v>240</v>
+      <c r="C94" s="1" t="s">
+        <v>357</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>311</v>
+        <v>363</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>224</v>
@@ -2988,18 +3009,18 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
+        <f t="shared" si="7"/>
+        <v>94</v>
+      </c>
+      <c r="B95" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>94</v>
-      </c>
-      <c r="B95" s="1" t="str">
-        <f t="shared" si="9"/>
         <v>Rule-094</v>
       </c>
       <c r="C95" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>224</v>
@@ -3007,18 +3028,18 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
+        <f t="shared" si="7"/>
+        <v>95</v>
+      </c>
+      <c r="B96" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>95</v>
-      </c>
-      <c r="B96" s="1" t="str">
-        <f t="shared" si="9"/>
         <v>Rule-095</v>
       </c>
       <c r="C96" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>224</v>
@@ -3026,37 +3047,37 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
+        <f t="shared" si="7"/>
+        <v>96</v>
+      </c>
+      <c r="B97" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>96</v>
-      </c>
-      <c r="B97" s="1" t="str">
-        <f t="shared" si="9"/>
         <v>Rule-096</v>
       </c>
       <c r="C97" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>307</v>
+        <v>289</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="98" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
+        <f t="shared" si="7"/>
+        <v>97</v>
+      </c>
+      <c r="B98" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>97</v>
-      </c>
-      <c r="B98" s="1" t="str">
-        <f t="shared" si="9"/>
         <v>Rule-097</v>
       </c>
-      <c r="C98" s="1" t="s">
-        <v>330</v>
+      <c r="C98" t="s">
+        <v>246</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>335</v>
+        <v>299</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>224</v>
@@ -3064,18 +3085,18 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
+        <f t="shared" si="7"/>
+        <v>98</v>
+      </c>
+      <c r="B99" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>98</v>
-      </c>
-      <c r="B99" s="1" t="str">
-        <f t="shared" si="9"/>
         <v>Rule-098</v>
       </c>
       <c r="C99" t="s">
-        <v>331</v>
-      </c>
-      <c r="D99" t="s">
-        <v>336</v>
+        <v>247</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>305</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>224</v>
@@ -3083,171 +3104,248 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
+        <f t="shared" si="7"/>
+        <v>99</v>
+      </c>
+      <c r="B100" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>99</v>
-      </c>
-      <c r="B100" s="1" t="str">
-        <f t="shared" ref="B100" si="10">CONCATENATE("Rule-",TEXT(A100,"000"))</f>
         <v>Rule-099</v>
       </c>
-      <c r="C100" t="s">
-        <v>250</v>
+      <c r="C100" s="1" t="s">
+        <v>358</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>314</v>
+        <v>364</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="101" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="1" t="s">
-        <v>357</v>
+      <c r="A101" s="1">
+        <f t="shared" si="7"/>
+        <v>100</v>
+      </c>
+      <c r="B101" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>Rule-100</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>339</v>
+        <v>328</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B102" s="1" t="s">
-        <v>357</v>
+      <c r="A102" s="1">
+        <f t="shared" si="7"/>
+        <v>101</v>
+      </c>
+      <c r="B102" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>Rule-101</v>
       </c>
       <c r="C102" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B103" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>341</v>
+        <v>329</v>
+      </c>
+      <c r="D102" t="s">
+        <v>334</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <f t="shared" si="7"/>
+        <v>102</v>
+      </c>
+      <c r="B103" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>Rule-102</v>
+      </c>
+      <c r="C103" t="s">
+        <v>248</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="104" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B104" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B105" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>355</v>
+      </c>
+      <c r="C105" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B106" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>344</v>
+        <v>359</v>
       </c>
     </row>
     <row r="107" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B107" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
     </row>
     <row r="108" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B108" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
     </row>
     <row r="109" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B109" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
     </row>
     <row r="110" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B110" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="111" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B111" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="112" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B112" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.25">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="113" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B113" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="C113" t="s">
-        <v>351</v>
-      </c>
-      <c r="F113" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.25">
+        <v>355</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="114" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B114" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="C114" t="s">
-        <v>352</v>
-      </c>
-      <c r="F114" s="1" t="s">
-        <v>237</v>
+        <v>355</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="115" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B115" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="C115" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.25">
+        <v>355</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="116" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B116" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="C116" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.25">
+        <v>355</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="117" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B117" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="C117" t="s">
         <v>355</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="118" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B118" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C118" t="s">
-        <v>356</v>
+        <v>349</v>
+      </c>
+      <c r="F118" s="1"/>
+    </row>
+    <row r="119" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B119" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C119" t="s">
+        <v>350</v>
+      </c>
+      <c r="F119" s="1"/>
+    </row>
+    <row r="120" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B120" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C120" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B121" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="122" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B122" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C122" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="123" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B123" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C123" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="124" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B124" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C124" t="s">
+        <v>354</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Content Manager role - ditamaps, common topics, main index.html, header, css. Added basic 'Building Your Site' topics. Added outputclass (class id) to separate formatting (bold) from role callouts and terms. Added the bold to the css instead. Tweaked title change in Security topics and references. Updates to css and logo from James Hellersen. Updated web.config. In ditamaps: 	* Consolidated the references into one section. 	* Added content manager stuff. 	* Updated reltables. Bug fixes.
</commit_message>
<xml_diff>
--- a/_build/urlmap/DC-URLmapping.xlsx
+++ b/_build/urlmap/DC-URLmapping.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="400">
   <si>
     <t>DNN8-Requirements.html</t>
   </si>
@@ -1008,27 +1008,9 @@
     <t>developers/security/jwt</t>
   </si>
   <si>
-    <t>administrators/security/index.html</t>
-  </si>
-  <si>
-    <t>administrators/security/jwt/index.html</t>
-  </si>
-  <si>
-    <t>administrators/security/roles/index.html</t>
-  </si>
-  <si>
-    <t>developers/security/index.html</t>
-  </si>
-  <si>
-    <t>developers/security/jwt/index.html</t>
-  </si>
-  <si>
     <t>/index.html</t>
   </si>
   <si>
-    <t>administrators/extensions/index.html</t>
-  </si>
-  <si>
     <t>administrators/</t>
   </si>
   <si>
@@ -1104,13 +1086,136 @@
     <t>developers/included-modules/</t>
   </si>
   <si>
-    <t>administrators/included-modules/index.html</t>
-  </si>
-  <si>
-    <t>designers/included-modules/index.html</t>
-  </si>
-  <si>
-    <t>developers/included-modules/index.html</t>
+    <t>administrators/security/user-accounts   administrators/security/user-accounts/index.html</t>
+  </si>
+  <si>
+    <t>content-managers/security/user-accounts content-managers/security/user-accounts/index.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  administrators/index.html</t>
+  </si>
+  <si>
+    <t>administrators/building-your-site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   administrators/building-your-site/index.html</t>
+  </si>
+  <si>
+    <t>administrators/configuration</t>
+  </si>
+  <si>
+    <t>administrators/configuration/index.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   administrators/extensions/index.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> administrators/included-modules/index.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> administrators/security/index.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> administrators/security/jwt/index.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   administrators/security/roles/index.html</t>
+  </si>
+  <si>
+    <t>content-managers</t>
+  </si>
+  <si>
+    <t>content-managers/index.html</t>
+  </si>
+  <si>
+    <t>content-managers/building-your-site</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> content-managers/building-your-site/index.html</t>
+  </si>
+  <si>
+    <t>content-managers/included-modules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   content-managers/included-modules/index.html</t>
+  </si>
+  <si>
+    <t>content-managers/security</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   content-managers/security/index.html</t>
+  </si>
+  <si>
+    <t>content-managers/security/roles</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> content-managers/security/roles/index.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   designers/index.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   designers/creating-themes/index.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  designers/included-modules/index.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> designers/setup/index.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  developers/index.html</t>
+  </si>
+  <si>
+    <t>developers/configuration</t>
+  </si>
+  <si>
+    <t>developers/configuration/index.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> developers/creating-modules/index.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   developers/extensions/index.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> developers/included-modules/index.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> developers/security/index.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> developers/security/jwt/index.html</t>
+  </si>
+  <si>
+    <t>administrators/building-your-site/</t>
+  </si>
+  <si>
+    <t>administrators/configuration/</t>
+  </si>
+  <si>
+    <t>administrators/security/user-accounts/</t>
+  </si>
+  <si>
+    <t>content-managers/</t>
+  </si>
+  <si>
+    <t>content-managers/building-your-site/</t>
+  </si>
+  <si>
+    <t>content-managers/included-modules/</t>
+  </si>
+  <si>
+    <t>content-managers/security/</t>
+  </si>
+  <si>
+    <t>content-managers/security/roles/</t>
+  </si>
+  <si>
+    <t>content-managers/security/user-accounts/</t>
+  </si>
+  <si>
+    <t>developers/configuration/</t>
   </si>
 </sst>
 </file>
@@ -1469,10 +1574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G124"/>
+  <dimension ref="A1:G144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B124" sqref="B2:D124"/>
+      <selection activeCell="B144" sqref="B2:D144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1512,7 +1617,7 @@
         <v>231</v>
       </c>
       <c r="D2" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>224</v>
@@ -2733,7 +2838,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <f t="shared" ref="A80:A103" si="7">A79+1</f>
+        <f t="shared" ref="A80:A113" si="7">A79+1</f>
         <v>79</v>
       </c>
       <c r="B80" s="1" t="str">
@@ -2792,7 +2897,7 @@
         <v>236</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>252</v>
+        <v>358</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>224</v>
@@ -2808,10 +2913,10 @@
         <v>Rule-083</v>
       </c>
       <c r="C84" t="s">
-        <v>239</v>
+        <v>359</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>336</v>
+        <v>360</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>224</v>
@@ -2827,7 +2932,7 @@
         <v>Rule-084</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>356</v>
+        <v>361</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>362</v>
@@ -2846,10 +2951,10 @@
         <v>Rule-085</v>
       </c>
       <c r="C86" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D86" t="s">
-        <v>256</v>
+        <v>363</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>224</v>
@@ -2865,10 +2970,10 @@
         <v>Rule-086</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>325</v>
+        <v>350</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>330</v>
+        <v>364</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>224</v>
@@ -2884,10 +2989,10 @@
         <v>Rule-087</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>326</v>
+        <v>240</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>331</v>
+        <v>256</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>224</v>
@@ -2903,10 +3008,10 @@
         <v>Rule-088</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>332</v>
+        <v>365</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>224</v>
@@ -2922,10 +3027,10 @@
         <v>Rule-089</v>
       </c>
       <c r="C90" t="s">
-        <v>241</v>
+        <v>326</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>260</v>
+        <v>366</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>224</v>
@@ -2941,10 +3046,10 @@
         <v>Rule-090</v>
       </c>
       <c r="C91" t="s">
-        <v>237</v>
+        <v>327</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>279</v>
+        <v>367</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>224</v>
@@ -2960,11 +3065,9 @@
         <v>Rule-091</v>
       </c>
       <c r="C92" t="s">
-        <v>242</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>272</v>
-      </c>
+        <v>356</v>
+      </c>
+      <c r="D92" s="1"/>
       <c r="F92" s="1" t="s">
         <v>224</v>
       </c>
@@ -2979,10 +3082,10 @@
         <v>Rule-092</v>
       </c>
       <c r="C93" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>224</v>
@@ -2998,10 +3101,10 @@
         <v>Rule-093</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>357</v>
+        <v>368</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>224</v>
@@ -3017,10 +3120,10 @@
         <v>Rule-094</v>
       </c>
       <c r="C95" t="s">
-        <v>244</v>
+        <v>370</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>281</v>
+        <v>371</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>224</v>
@@ -3036,10 +3139,10 @@
         <v>Rule-095</v>
       </c>
       <c r="C96" t="s">
-        <v>238</v>
+        <v>372</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>309</v>
+        <v>373</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>224</v>
@@ -3055,10 +3158,10 @@
         <v>Rule-096</v>
       </c>
       <c r="C97" t="s">
-        <v>245</v>
+        <v>374</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>289</v>
+        <v>375</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>224</v>
@@ -3074,10 +3177,10 @@
         <v>Rule-097</v>
       </c>
       <c r="C98" t="s">
-        <v>246</v>
+        <v>376</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>299</v>
+        <v>377</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>224</v>
@@ -3093,11 +3196,9 @@
         <v>Rule-098</v>
       </c>
       <c r="C99" t="s">
-        <v>247</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>305</v>
-      </c>
+        <v>357</v>
+      </c>
+      <c r="D99" s="1"/>
       <c r="F99" s="1" t="s">
         <v>224</v>
       </c>
@@ -3112,10 +3213,10 @@
         <v>Rule-099</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>358</v>
+        <v>237</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>364</v>
+        <v>378</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>224</v>
@@ -3131,10 +3232,10 @@
         <v>Rule-100</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>328</v>
+        <v>242</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>333</v>
+        <v>379</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>224</v>
@@ -3150,10 +3251,10 @@
         <v>Rule-101</v>
       </c>
       <c r="C102" t="s">
-        <v>329</v>
+        <v>243</v>
       </c>
       <c r="D102" t="s">
-        <v>334</v>
+        <v>275</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>224</v>
@@ -3169,183 +3270,453 @@
         <v>Rule-102</v>
       </c>
       <c r="C103" t="s">
-        <v>248</v>
+        <v>351</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>312</v>
+        <v>380</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="104" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="1" t="s">
+      <c r="A104" s="1">
+        <f t="shared" si="7"/>
+        <v>103</v>
+      </c>
+      <c r="B104" s="1" t="str">
+        <f t="shared" ref="B104:B113" si="9">CONCATENATE("Rule-",TEXT(A104,"000"))</f>
+        <v>Rule-103</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <f t="shared" si="7"/>
+        <v>104</v>
+      </c>
+      <c r="B105" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>Rule-104</v>
+      </c>
+      <c r="C105" t="s">
+        <v>238</v>
+      </c>
+      <c r="D105" t="s">
+        <v>382</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <f t="shared" si="7"/>
+        <v>105</v>
+      </c>
+      <c r="B106" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>Rule-105</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D106" t="s">
+        <v>289</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <f t="shared" si="7"/>
+        <v>106</v>
+      </c>
+      <c r="B107" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>Rule-106</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
+        <f t="shared" si="7"/>
+        <v>107</v>
+      </c>
+      <c r="B108" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>Rule-107</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <f t="shared" si="7"/>
+        <v>108</v>
+      </c>
+      <c r="B109" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>Rule-108</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <f t="shared" si="7"/>
+        <v>109</v>
+      </c>
+      <c r="B110" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>Rule-109</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <f t="shared" si="7"/>
+        <v>110</v>
+      </c>
+      <c r="B111" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>Rule-110</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
+        <f t="shared" si="7"/>
+        <v>111</v>
+      </c>
+      <c r="B112" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>Rule-111</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
+        <f t="shared" si="7"/>
+        <v>112</v>
+      </c>
+      <c r="B113" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>Rule-112</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B114" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B115" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B116" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B117" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B118" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C118" t="s">
+        <v>353</v>
+      </c>
+      <c r="F118" s="1"/>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B119" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C119" t="s">
+        <v>333</v>
+      </c>
+      <c r="F119" s="1"/>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B120" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C120" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B121" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B122" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C122" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B123" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C123" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B124" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C124" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B125" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C125" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B126" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C126" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B127" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C127" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B128" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C128" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B129" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C129" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B130" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C130" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B131" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C131" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B132" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C132" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B133" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C133" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B134" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C134" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B135" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C135" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B136" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C136" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B137" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C137" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B138" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C138" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B139" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C139" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B140" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C140" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B141" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C141" t="s">
         <v>355</v>
       </c>
-      <c r="C104" s="1" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B105" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C105" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B106" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B107" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B108" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B109" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B110" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B111" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B112" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="113" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B113" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="114" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B114" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C114" s="1" t="s">
+    </row>
+    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B142" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C142" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B115" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="116" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B116" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C116" s="1" t="s">
+    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B143" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C143" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="117" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B117" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C117" s="1" t="s">
+    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B144" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C144" t="s">
         <v>348</v>
-      </c>
-    </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B118" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C118" t="s">
-        <v>349</v>
-      </c>
-      <c r="F118" s="1"/>
-    </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B119" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C119" t="s">
-        <v>350</v>
-      </c>
-      <c r="F119" s="1"/>
-    </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B120" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C120" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B121" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B122" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C122" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B123" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C123" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B124" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C124" t="s">
-        <v>354</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replaced role icons with svg files from Sam Sze. Updated web.config.
</commit_message>
<xml_diff>
--- a/_build/urlmap/DC-URLmapping.xlsx
+++ b/_build/urlmap/DC-URLmapping.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="416">
   <si>
     <t>DNN8-Requirements.html</t>
   </si>
@@ -1086,42 +1086,15 @@
     <t>developers/included-modules/</t>
   </si>
   <si>
-    <t>administrators/security/user-accounts   administrators/security/user-accounts/index.html</t>
-  </si>
-  <si>
-    <t>content-managers/security/user-accounts content-managers/security/user-accounts/index.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  administrators/index.html</t>
-  </si>
-  <si>
     <t>administrators/building-your-site</t>
   </si>
   <si>
-    <t xml:space="preserve">   administrators/building-your-site/index.html</t>
-  </si>
-  <si>
     <t>administrators/configuration</t>
   </si>
   <si>
     <t>administrators/configuration/index.html</t>
   </si>
   <si>
-    <t xml:space="preserve">   administrators/extensions/index.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> administrators/included-modules/index.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> administrators/security/index.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> administrators/security/jwt/index.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   administrators/security/roles/index.html</t>
-  </si>
-  <si>
     <t>content-managers</t>
   </si>
   <si>
@@ -1131,63 +1104,21 @@
     <t>content-managers/building-your-site</t>
   </si>
   <si>
-    <t xml:space="preserve"> content-managers/building-your-site/index.html</t>
-  </si>
-  <si>
     <t>content-managers/included-modules</t>
   </si>
   <si>
-    <t xml:space="preserve">   content-managers/included-modules/index.html</t>
-  </si>
-  <si>
     <t>content-managers/security</t>
   </si>
   <si>
-    <t xml:space="preserve">   content-managers/security/index.html</t>
-  </si>
-  <si>
     <t>content-managers/security/roles</t>
   </si>
   <si>
-    <t xml:space="preserve"> content-managers/security/roles/index.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   designers/index.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   designers/creating-themes/index.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  designers/included-modules/index.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> designers/setup/index.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  developers/index.html</t>
-  </si>
-  <si>
     <t>developers/configuration</t>
   </si>
   <si>
     <t>developers/configuration/index.html</t>
   </si>
   <si>
-    <t xml:space="preserve"> developers/creating-modules/index.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   developers/extensions/index.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> developers/included-modules/index.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> developers/security/index.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> developers/security/jwt/index.html</t>
-  </si>
-  <si>
     <t>administrators/building-your-site/</t>
   </si>
   <si>
@@ -1216,6 +1147,123 @@
   </si>
   <si>
     <t>developers/configuration/</t>
+  </si>
+  <si>
+    <t>community-managers</t>
+  </si>
+  <si>
+    <t>administrators/building-your-site/index.html</t>
+  </si>
+  <si>
+    <t>administrators/extensions/index.html</t>
+  </si>
+  <si>
+    <t>administrators/included-modules/index.html</t>
+  </si>
+  <si>
+    <t>administrators/security/index.html</t>
+  </si>
+  <si>
+    <t>administrators/security/jwt/index.html</t>
+  </si>
+  <si>
+    <t>administrators/security/roles/index.html</t>
+  </si>
+  <si>
+    <t>administrators/security/user-accounts</t>
+  </si>
+  <si>
+    <t>administrators/security/user-accounts/index.html</t>
+  </si>
+  <si>
+    <t>community-managers/index.html</t>
+  </si>
+  <si>
+    <t>community-managers/included-modules</t>
+  </si>
+  <si>
+    <t>community-managers/included-modules/index.html</t>
+  </si>
+  <si>
+    <t>community-managers/managing-your-community</t>
+  </si>
+  <si>
+    <t>community-managers/managing-your-community/index.html</t>
+  </si>
+  <si>
+    <t>community-managers/security</t>
+  </si>
+  <si>
+    <t>community-managers/security/index.html</t>
+  </si>
+  <si>
+    <t>community-managers/security/roles</t>
+  </si>
+  <si>
+    <t>community-managers/security/roles/index.html</t>
+  </si>
+  <si>
+    <t>community-managers/security/user-accounts</t>
+  </si>
+  <si>
+    <t>community-managers/security/user-accounts/index.html</t>
+  </si>
+  <si>
+    <t>content-managers/building-your-site/index.html</t>
+  </si>
+  <si>
+    <t>content-managers/extensions</t>
+  </si>
+  <si>
+    <t>content-managers/extensions/index.html</t>
+  </si>
+  <si>
+    <t>content-managers/included-modules/index.html</t>
+  </si>
+  <si>
+    <t>content-managers/security/index.html</t>
+  </si>
+  <si>
+    <t>content-managers/security/roles/index.html</t>
+  </si>
+  <si>
+    <t>content-managers/security/user-accounts</t>
+  </si>
+  <si>
+    <t>content-managers/security/user-accounts/index.html</t>
+  </si>
+  <si>
+    <t>designers/included-modules/index.html</t>
+  </si>
+  <si>
+    <t>developers/included-modules/index.html</t>
+  </si>
+  <si>
+    <t>developers/security/index.html</t>
+  </si>
+  <si>
+    <t>developers/security/jwt/index.html</t>
+  </si>
+  <si>
+    <t>community-managers/</t>
+  </si>
+  <si>
+    <t>community-managers/included-modules/</t>
+  </si>
+  <si>
+    <t>community-managers/managing-your-community/</t>
+  </si>
+  <si>
+    <t>community-managers/security/</t>
+  </si>
+  <si>
+    <t>community-managers/security/roles/</t>
+  </si>
+  <si>
+    <t>community-managers/security/user-accounts/</t>
+  </si>
+  <si>
+    <t>content-managers/extensions/</t>
   </si>
 </sst>
 </file>
@@ -1574,16 +1622,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G144"/>
+  <dimension ref="A1:G158"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B144" sqref="B2:D144"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="C121" sqref="C121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="71.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="89" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="63.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="28.5703125" bestFit="1" customWidth="1"/>
@@ -2838,7 +2886,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <f t="shared" ref="A80:A113" si="7">A79+1</f>
+        <f t="shared" ref="A80:A120" si="7">A79+1</f>
         <v>79</v>
       </c>
       <c r="B80" s="1" t="str">
@@ -2897,7 +2945,7 @@
         <v>236</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>358</v>
+        <v>252</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>224</v>
@@ -2913,10 +2961,10 @@
         <v>Rule-083</v>
       </c>
       <c r="C84" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>360</v>
+        <v>378</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>224</v>
@@ -2932,10 +2980,10 @@
         <v>Rule-084</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>224</v>
@@ -2954,7 +3002,7 @@
         <v>239</v>
       </c>
       <c r="D86" t="s">
-        <v>363</v>
+        <v>379</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>224</v>
@@ -2973,7 +3021,7 @@
         <v>350</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>364</v>
+        <v>380</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>224</v>
@@ -3011,7 +3059,7 @@
         <v>325</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>365</v>
+        <v>381</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>224</v>
@@ -3030,7 +3078,7 @@
         <v>326</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>366</v>
+        <v>382</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>224</v>
@@ -3049,7 +3097,7 @@
         <v>327</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>367</v>
+        <v>383</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>224</v>
@@ -3065,9 +3113,11 @@
         <v>Rule-091</v>
       </c>
       <c r="C92" t="s">
-        <v>356</v>
-      </c>
-      <c r="D92" s="1"/>
+        <v>384</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>385</v>
+      </c>
       <c r="F92" s="1" t="s">
         <v>224</v>
       </c>
@@ -3101,10 +3151,10 @@
         <v>Rule-093</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>368</v>
+        <v>377</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>369</v>
+        <v>386</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>224</v>
@@ -3120,10 +3170,10 @@
         <v>Rule-094</v>
       </c>
       <c r="C95" t="s">
-        <v>370</v>
+        <v>387</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>371</v>
+        <v>388</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>224</v>
@@ -3139,10 +3189,10 @@
         <v>Rule-095</v>
       </c>
       <c r="C96" t="s">
-        <v>372</v>
+        <v>389</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>373</v>
+        <v>390</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>224</v>
@@ -3158,10 +3208,10 @@
         <v>Rule-096</v>
       </c>
       <c r="C97" t="s">
-        <v>374</v>
+        <v>391</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>375</v>
+        <v>392</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>224</v>
@@ -3177,10 +3227,10 @@
         <v>Rule-097</v>
       </c>
       <c r="C98" t="s">
-        <v>376</v>
+        <v>393</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>377</v>
+        <v>394</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>224</v>
@@ -3196,9 +3246,11 @@
         <v>Rule-098</v>
       </c>
       <c r="C99" t="s">
-        <v>357</v>
-      </c>
-      <c r="D99" s="1"/>
+        <v>395</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>396</v>
+      </c>
       <c r="F99" s="1" t="s">
         <v>224</v>
       </c>
@@ -3213,10 +3265,10 @@
         <v>Rule-099</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>237</v>
+        <v>359</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>378</v>
+        <v>360</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>224</v>
@@ -3232,10 +3284,10 @@
         <v>Rule-100</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>242</v>
+        <v>361</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>379</v>
+        <v>397</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>224</v>
@@ -3251,10 +3303,10 @@
         <v>Rule-101</v>
       </c>
       <c r="C102" t="s">
-        <v>243</v>
+        <v>398</v>
       </c>
       <c r="D102" t="s">
-        <v>275</v>
+        <v>399</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>224</v>
@@ -3270,10 +3322,10 @@
         <v>Rule-102</v>
       </c>
       <c r="C103" t="s">
-        <v>351</v>
+        <v>362</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>380</v>
+        <v>400</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>224</v>
@@ -3289,10 +3341,10 @@
         <v>Rule-103</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>244</v>
+        <v>363</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>381</v>
+        <v>401</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>224</v>
@@ -3308,10 +3360,10 @@
         <v>Rule-104</v>
       </c>
       <c r="C105" t="s">
-        <v>238</v>
+        <v>364</v>
       </c>
       <c r="D105" t="s">
-        <v>382</v>
+        <v>402</v>
       </c>
       <c r="F105" s="1" t="s">
         <v>224</v>
@@ -3327,10 +3379,10 @@
         <v>Rule-105</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>245</v>
+        <v>403</v>
       </c>
       <c r="D106" t="s">
-        <v>289</v>
+        <v>404</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>224</v>
@@ -3346,10 +3398,10 @@
         <v>Rule-106</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>383</v>
+        <v>237</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>384</v>
+        <v>279</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>224</v>
@@ -3365,10 +3417,10 @@
         <v>Rule-107</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>385</v>
+        <v>272</v>
       </c>
       <c r="F108" s="1" t="s">
         <v>224</v>
@@ -3384,10 +3436,10 @@
         <v>Rule-108</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>386</v>
+        <v>275</v>
       </c>
       <c r="F109" s="1" t="s">
         <v>224</v>
@@ -3403,10 +3455,10 @@
         <v>Rule-109</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>387</v>
+        <v>405</v>
       </c>
       <c r="F110" s="1" t="s">
         <v>224</v>
@@ -3422,10 +3474,10 @@
         <v>Rule-110</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>328</v>
+        <v>244</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>388</v>
+        <v>281</v>
       </c>
       <c r="F111" s="1" t="s">
         <v>224</v>
@@ -3441,10 +3493,10 @@
         <v>Rule-111</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>329</v>
+        <v>238</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>389</v>
+        <v>309</v>
       </c>
       <c r="F112" s="1" t="s">
         <v>224</v>
@@ -3460,262 +3512,451 @@
         <v>Rule-112</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>312</v>
+        <v>289</v>
       </c>
       <c r="F113" s="1" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="114" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B114" s="1" t="s">
-        <v>349</v>
+      <c r="A114" s="1">
+        <f t="shared" si="7"/>
+        <v>113</v>
+      </c>
+      <c r="B114" s="1" t="str">
+        <f t="shared" ref="B114:B120" si="10">CONCATENATE("Rule-",TEXT(A114,"000"))</f>
+        <v>Rule-113</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B115" s="1" t="s">
-        <v>349</v>
+        <v>365</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <f t="shared" si="7"/>
+        <v>114</v>
+      </c>
+      <c r="B115" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>Rule-114</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>390</v>
+        <v>246</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="116" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B116" s="1" t="s">
-        <v>349</v>
+      <c r="A116" s="1">
+        <f t="shared" si="7"/>
+        <v>115</v>
+      </c>
+      <c r="B116" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>Rule-115</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>391</v>
+        <v>247</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="117" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B117" s="1" t="s">
-        <v>349</v>
+      <c r="A117" s="1">
+        <f t="shared" si="7"/>
+        <v>116</v>
+      </c>
+      <c r="B117" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>Rule-116</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B118" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="C118" t="s">
-        <v>353</v>
-      </c>
-      <c r="F118" s="1"/>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B119" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="C119" t="s">
-        <v>333</v>
-      </c>
-      <c r="F119" s="1"/>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B120" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="C120" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="1">
+        <f t="shared" si="7"/>
+        <v>117</v>
+      </c>
+      <c r="B118" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>Rule-117</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
+        <f t="shared" si="7"/>
+        <v>118</v>
+      </c>
+      <c r="B119" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>Rule-118</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
+        <f t="shared" si="7"/>
+        <v>119</v>
+      </c>
+      <c r="B120" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>Rule-119</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B121" s="1" t="s">
         <v>349</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B122" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="C122" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C122" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B123" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="C123" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C123" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B124" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="C124" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C124" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B125" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="C125" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C125" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B126" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="C126" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C126" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B127" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="C127" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C127" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B128" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="C128" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C128" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="129" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B129" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="C129" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C129" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="130" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B130" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="C130" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C130" s="1" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="131" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B131" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="C131" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C131" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="132" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B132" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="C132" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C132" s="1" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="133" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B133" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="C133" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C133" s="1" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="134" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B134" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="C134" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C134" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="135" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B135" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="C135" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C135" s="1" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="136" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B136" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="C136" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C136" s="1" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="137" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B137" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="C137" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C137" s="1" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="138" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B138" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="C138" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C138" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="139" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B139" s="1" t="s">
         <v>349</v>
       </c>
       <c r="C139" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
+        <v>371</v>
+      </c>
+      <c r="F139" s="1"/>
+    </row>
+    <row r="140" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B140" s="1" t="s">
         <v>349</v>
       </c>
       <c r="C140" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
+        <v>415</v>
+      </c>
+      <c r="F140" s="1"/>
+    </row>
+    <row r="141" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B141" s="1" t="s">
         <v>349</v>
       </c>
       <c r="C141" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="142" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B142" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="C142" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C142" s="1" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="143" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B143" s="1" t="s">
         <v>349</v>
       </c>
       <c r="C143" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="144" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B144" s="1" t="s">
         <v>349</v>
       </c>
       <c r="C144" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B145" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C145" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B146" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C146" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="147" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B147" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C147" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="148" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B148" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C148" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="149" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B149" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C149" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="150" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B150" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C150" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="151" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B151" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C151" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="152" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B152" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C152" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="153" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B153" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C153" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="154" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B154" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C154" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="155" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B155" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C155" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="156" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B156" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C156" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="157" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B157" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C157" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="158" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B158" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C158" t="s">
         <v>348</v>
       </c>
     </row>

</xml_diff>

<commit_message>
* Changed the build to automatically update the web.config when new subdirectories are added. * Added product logos to most of the pages. (James updated the CSS to make the logos line up to the right of the title, but still need to add the CSS versioning to the DITA build.) * Replaced strict task topics with general task topics.
</commit_message>
<xml_diff>
--- a/_build/urlmap/DC-URLmapping.xlsx
+++ b/_build/urlmap/DC-URLmapping.xlsx
@@ -7,16 +7,17 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="20160325 old2new" sheetId="5" r:id="rId1"/>
-    <sheet name="20160323 old2new" sheetId="2" r:id="rId2"/>
-    <sheet name="20160309 old2new" sheetId="4" r:id="rId3"/>
+    <sheet name="20160701 old2new" sheetId="6" r:id="rId1"/>
+    <sheet name="20160325 old2new" sheetId="5" r:id="rId2"/>
+    <sheet name="20160323 old2new" sheetId="2" r:id="rId3"/>
+    <sheet name="20160309 old2new" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="418">
   <si>
     <t>DNN8-Requirements.html</t>
   </si>
@@ -1264,6 +1265,12 @@
   </si>
   <si>
     <t>content-managers/extensions/</t>
+  </si>
+  <si>
+    <t>old</t>
+  </si>
+  <si>
+    <t>new</t>
   </si>
 </sst>
 </file>
@@ -1322,7 +1329,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1411,6 +1424,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1446,6 +1476,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1622,10 +1669,548 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="89" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="71.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="C121" sqref="C121"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1673,12 +2258,12 @@
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <f>A2+1</f>
-        <v>2</v>
+        <f>IF(C3="",A2,A2+1)</f>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="str">
         <f t="shared" ref="B3" si="0">CONCATENATE("Rule-",TEXT(A3,"000"))</f>
-        <v>Rule-002</v>
+        <v>Rule-001</v>
       </c>
       <c r="D3" t="s">
         <v>249</v>
@@ -1686,12 +2271,12 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:A8" si="1">A3+1</f>
-        <v>3</v>
+        <f t="shared" ref="A4:A67" si="1">IF(C4="",A3,A3+1)</f>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="str">
         <f>CONCATENATE("Rule-",TEXT(A4,"000"))</f>
-        <v>Rule-003</v>
+        <v>Rule-002</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>1</v>
@@ -1706,11 +2291,11 @@
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="str">
         <f t="shared" ref="B5:B17" si="2">CONCATENATE("Rule-",TEXT(A5,"000"))</f>
-        <v>Rule-004</v>
+        <v>Rule-003</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>2</v>
@@ -1726,11 +2311,11 @@
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>Rule-005</v>
+        <v>Rule-004</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>0</v>
@@ -1746,11 +2331,11 @@
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>Rule-006</v>
+        <v>Rule-005</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
@@ -1762,11 +2347,11 @@
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>Rule-007</v>
+        <v>Rule-006</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>10</v>
@@ -1778,12 +2363,12 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <f t="shared" ref="A9:A67" si="3">A8+1</f>
-        <v>8</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>Rule-008</v>
+        <v>Rule-007</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>12</v>
@@ -1794,12 +2379,12 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <f t="shared" si="3"/>
-        <v>9</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
       <c r="B10" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>Rule-009</v>
+        <v>Rule-007</v>
       </c>
       <c r="D10" t="s">
         <v>253</v>
@@ -1807,12 +2392,12 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <f t="shared" si="3"/>
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
       <c r="B11" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>Rule-010</v>
+        <v>Rule-007</v>
       </c>
       <c r="D11" t="s">
         <v>254</v>
@@ -1821,12 +2406,12 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <f t="shared" si="3"/>
-        <v>11</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
       <c r="B12" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>Rule-011</v>
+        <v>Rule-007</v>
       </c>
       <c r="D12" t="s">
         <v>255</v>
@@ -1834,12 +2419,12 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <f t="shared" si="3"/>
-        <v>12</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
       <c r="B13" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>Rule-012</v>
+        <v>Rule-007</v>
       </c>
       <c r="D13" t="s">
         <v>256</v>
@@ -1848,12 +2433,12 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <f t="shared" si="3"/>
-        <v>13</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
       <c r="B14" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>Rule-013</v>
+        <v>Rule-007</v>
       </c>
       <c r="D14" t="s">
         <v>257</v>
@@ -1862,12 +2447,12 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <f t="shared" si="3"/>
-        <v>14</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
       <c r="B15" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>Rule-014</v>
+        <v>Rule-007</v>
       </c>
       <c r="D15" t="s">
         <v>258</v>
@@ -1876,12 +2461,12 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <f t="shared" si="3"/>
-        <v>15</v>
+        <f t="shared" si="1"/>
+        <v>8</v>
       </c>
       <c r="B16" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>Rule-015</v>
+        <v>Rule-008</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>3</v>
@@ -1893,12 +2478,12 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <f t="shared" si="3"/>
-        <v>16</v>
+        <f t="shared" si="1"/>
+        <v>9</v>
       </c>
       <c r="B17" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>Rule-016</v>
+        <v>Rule-009</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>6</v>
@@ -1910,12 +2495,12 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <f t="shared" si="3"/>
-        <v>17</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="B18" s="1" t="str">
-        <f t="shared" ref="B18:B67" si="4">CONCATENATE("Rule-",TEXT(A18,"000"))</f>
-        <v>Rule-017</v>
+        <f t="shared" ref="B18:B67" si="3">CONCATENATE("Rule-",TEXT(A18,"000"))</f>
+        <v>Rule-010</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>7</v>
@@ -1926,12 +2511,12 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B19" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>18</v>
-      </c>
-      <c r="B19" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-018</v>
+        <v>Rule-011</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>5</v>
@@ -1942,12 +2527,12 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B20" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>19</v>
-      </c>
-      <c r="B20" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-019</v>
+        <v>Rule-012</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>8</v>
@@ -1958,12 +2543,12 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B21" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="B21" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-020</v>
+        <v>Rule-013</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>9</v>
@@ -1974,12 +2559,12 @@
     </row>
     <row r="22" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B22" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>21</v>
-      </c>
-      <c r="B22" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-021</v>
+        <v>Rule-014</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>11</v>
@@ -1993,12 +2578,12 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B23" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>22</v>
-      </c>
-      <c r="B23" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-022</v>
+        <v>Rule-014</v>
       </c>
       <c r="D23" t="s">
         <v>266</v>
@@ -2006,12 +2591,12 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B24" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>23</v>
-      </c>
-      <c r="B24" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-023</v>
+        <v>Rule-015</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>22</v>
@@ -2022,12 +2607,12 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B25" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>24</v>
-      </c>
-      <c r="B25" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-024</v>
+        <v>Rule-016</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>21</v>
@@ -2038,12 +2623,12 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B26" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>25</v>
-      </c>
-      <c r="B26" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-025</v>
+        <v>Rule-017</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>23</v>
@@ -2055,12 +2640,12 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B27" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>26</v>
-      </c>
-      <c r="B27" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-026</v>
+        <v>Rule-018</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>24</v>
@@ -2072,12 +2657,12 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="B28" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>27</v>
-      </c>
-      <c r="B28" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-027</v>
+        <v>Rule-019</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>25</v>
@@ -2089,12 +2674,12 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B29" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>28</v>
-      </c>
-      <c r="B29" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-028</v>
+        <v>Rule-020</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>27</v>
@@ -2106,12 +2691,12 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B30" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>29</v>
-      </c>
-      <c r="B30" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-029</v>
+        <v>Rule-020</v>
       </c>
       <c r="D30" t="s">
         <v>273</v>
@@ -2119,12 +2704,12 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B31" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>30</v>
-      </c>
-      <c r="B31" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-030</v>
+        <v>Rule-020</v>
       </c>
       <c r="D31" t="s">
         <v>321</v>
@@ -2132,12 +2717,12 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="B32" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>31</v>
-      </c>
-      <c r="B32" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-031</v>
+        <v>Rule-021</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>29</v>
@@ -2149,12 +2734,12 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="B33" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>32</v>
-      </c>
-      <c r="B33" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-032</v>
+        <v>Rule-022</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>30</v>
@@ -2166,12 +2751,12 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="B34" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>33</v>
-      </c>
-      <c r="B34" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-033</v>
+        <v>Rule-023</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>14</v>
@@ -2182,12 +2767,12 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="B35" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>34</v>
-      </c>
-      <c r="B35" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-034</v>
+        <v>Rule-024</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>28</v>
@@ -2198,12 +2783,12 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="B36" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>35</v>
-      </c>
-      <c r="B36" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-035</v>
+        <v>Rule-025</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>20</v>
@@ -2214,12 +2799,12 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="B37" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>36</v>
-      </c>
-      <c r="B37" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-036</v>
+        <v>Rule-026</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>33</v>
@@ -2230,12 +2815,12 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="B38" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>37</v>
-      </c>
-      <c r="B38" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-037</v>
+        <v>Rule-026</v>
       </c>
       <c r="D38" t="s">
         <v>323</v>
@@ -2243,12 +2828,12 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="B39" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>38</v>
-      </c>
-      <c r="B39" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-038</v>
+        <v>Rule-026</v>
       </c>
       <c r="D39" t="s">
         <v>280</v>
@@ -2256,12 +2841,12 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="B40" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>39</v>
-      </c>
-      <c r="B40" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-039</v>
+        <v>Rule-027</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>13</v>
@@ -2272,12 +2857,12 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="B41" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>40</v>
-      </c>
-      <c r="B41" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-040</v>
+        <v>Rule-028</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>16</v>
@@ -2288,12 +2873,12 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="B42" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>41</v>
-      </c>
-      <c r="B42" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-041</v>
+        <v>Rule-029</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>17</v>
@@ -2304,12 +2889,12 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="B43" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>42</v>
-      </c>
-      <c r="B43" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-042</v>
+        <v>Rule-030</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>15</v>
@@ -2320,12 +2905,12 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="B44" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>43</v>
-      </c>
-      <c r="B44" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-043</v>
+        <v>Rule-031</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>18</v>
@@ -2336,12 +2921,12 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="B45" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>44</v>
-      </c>
-      <c r="B45" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-044</v>
+        <v>Rule-032</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>19</v>
@@ -2352,12 +2937,12 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="B46" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>45</v>
-      </c>
-      <c r="B46" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-045</v>
+        <v>Rule-033</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>32</v>
@@ -2368,12 +2953,12 @@
     </row>
     <row r="47" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="B47" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>46</v>
-      </c>
-      <c r="B47" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-046</v>
+        <v>Rule-034</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>31</v>
@@ -2387,12 +2972,12 @@
     </row>
     <row r="48" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="B48" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>47</v>
-      </c>
-      <c r="B48" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-047</v>
+        <v>Rule-035</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>26</v>
@@ -2406,12 +2991,12 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="B49" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>48</v>
-      </c>
-      <c r="B49" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-048</v>
+        <v>Rule-035</v>
       </c>
       <c r="D49" t="s">
         <v>288</v>
@@ -2419,12 +3004,12 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="B50" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>49</v>
-      </c>
-      <c r="B50" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-049</v>
+        <v>Rule-036</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>35</v>
@@ -2435,12 +3020,12 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="B51" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>50</v>
-      </c>
-      <c r="B51" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-050</v>
+        <v>Rule-037</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>38</v>
@@ -2451,12 +3036,12 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="B52" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>51</v>
-      </c>
-      <c r="B52" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-051</v>
+        <v>Rule-038</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>36</v>
@@ -2467,12 +3052,12 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="B53" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>52</v>
-      </c>
-      <c r="B53" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-052</v>
+        <v>Rule-039</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>39</v>
@@ -2483,12 +3068,12 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="B54" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>53</v>
-      </c>
-      <c r="B54" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-053</v>
+        <v>Rule-040</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>37</v>
@@ -2499,12 +3084,12 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="B55" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>54</v>
-      </c>
-      <c r="B55" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-054</v>
+        <v>Rule-041</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>40</v>
@@ -2516,12 +3101,12 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="B56" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>55</v>
-      </c>
-      <c r="B56" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-055</v>
+        <v>Rule-042</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>41</v>
@@ -2533,12 +3118,12 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="B57" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>56</v>
-      </c>
-      <c r="B57" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-056</v>
+        <v>Rule-043</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>42</v>
@@ -2550,12 +3135,12 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="B58" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>57</v>
-      </c>
-      <c r="B58" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-057</v>
+        <v>Rule-044</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>51</v>
@@ -2566,12 +3151,12 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="B59" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>58</v>
-      </c>
-      <c r="B59" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-058</v>
+        <v>Rule-045</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>52</v>
@@ -2582,12 +3167,12 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="B60" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>59</v>
-      </c>
-      <c r="B60" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-059</v>
+        <v>Rule-046</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>54</v>
@@ -2599,12 +3184,12 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="B61" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>60</v>
-      </c>
-      <c r="B61" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-060</v>
+        <v>Rule-046</v>
       </c>
       <c r="D61" t="s">
         <v>300</v>
@@ -2613,12 +3198,12 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="B62" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>61</v>
-      </c>
-      <c r="B62" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-061</v>
+        <v>Rule-046</v>
       </c>
       <c r="D62" t="s">
         <v>301</v>
@@ -2627,12 +3212,12 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="B63" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>62</v>
-      </c>
-      <c r="B63" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-062</v>
+        <v>Rule-047</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>53</v>
@@ -2643,12 +3228,12 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="B64" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>63</v>
-      </c>
-      <c r="B64" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-063</v>
+        <v>Rule-047</v>
       </c>
       <c r="D64" t="s">
         <v>303</v>
@@ -2656,12 +3241,12 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="B65" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>64</v>
-      </c>
-      <c r="B65" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-064</v>
+        <v>Rule-047</v>
       </c>
       <c r="D65" t="s">
         <v>322</v>
@@ -2669,12 +3254,12 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="B66" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>65</v>
-      </c>
-      <c r="B66" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-065</v>
+        <v>Rule-048</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>56</v>
@@ -2685,12 +3270,12 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="B67" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>66</v>
-      </c>
-      <c r="B67" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Rule-066</v>
+        <v>Rule-049</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>57</v>
@@ -2701,12 +3286,12 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <f t="shared" ref="A68:A79" si="5">A67+1</f>
-        <v>67</v>
+        <f t="shared" ref="A68:A120" si="4">IF(C68="",A67,A67+1)</f>
+        <v>50</v>
       </c>
       <c r="B68" s="1" t="str">
-        <f t="shared" ref="B68:B81" si="6">CONCATENATE("Rule-",TEXT(A68,"000"))</f>
-        <v>Rule-067</v>
+        <f t="shared" ref="B68:B81" si="5">CONCATENATE("Rule-",TEXT(A68,"000"))</f>
+        <v>Rule-050</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>44</v>
@@ -2717,932 +3302,932 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
+        <f t="shared" si="4"/>
+        <v>51</v>
+      </c>
+      <c r="B69" s="1" t="str">
         <f t="shared" si="5"/>
+        <v>Rule-051</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D69" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <f t="shared" si="4"/>
+        <v>52</v>
+      </c>
+      <c r="B70" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Rule-052</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D70" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <f t="shared" si="4"/>
+        <v>53</v>
+      </c>
+      <c r="B71" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Rule-053</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D71" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <f t="shared" si="4"/>
+        <v>53</v>
+      </c>
+      <c r="B72" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Rule-053</v>
+      </c>
+      <c r="D72" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <f t="shared" si="4"/>
+        <v>53</v>
+      </c>
+      <c r="B73" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Rule-053</v>
+      </c>
+      <c r="D73" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <f t="shared" si="4"/>
+        <v>53</v>
+      </c>
+      <c r="B74" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Rule-053</v>
+      </c>
+      <c r="D74" t="s">
+        <v>311</v>
+      </c>
+      <c r="G74" s="1"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <f t="shared" si="4"/>
+        <v>54</v>
+      </c>
+      <c r="B75" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Rule-054</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D75" t="s">
+        <v>312</v>
+      </c>
+      <c r="G75" s="1"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <f t="shared" si="4"/>
+        <v>55</v>
+      </c>
+      <c r="B76" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Rule-055</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D76" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <f t="shared" si="4"/>
+        <v>56</v>
+      </c>
+      <c r="B77" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Rule-056</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D77" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <f t="shared" si="4"/>
+        <v>57</v>
+      </c>
+      <c r="B78" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Rule-057</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D78" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <f t="shared" si="4"/>
+        <v>58</v>
+      </c>
+      <c r="B79" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Rule-058</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D79" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <f t="shared" si="4"/>
+        <v>59</v>
+      </c>
+      <c r="B80" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Rule-059</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D80" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+      <c r="B81" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Rule-060</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+      <c r="B82" s="1" t="str">
+        <f t="shared" ref="B82:B103" si="6">CONCATENATE("Rule-",TEXT(A82,"000"))</f>
+        <v>Rule-060</v>
+      </c>
+      <c r="D82" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <f t="shared" si="4"/>
+        <v>61</v>
+      </c>
+      <c r="B83" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Rule-061</v>
+      </c>
+      <c r="C83" t="s">
+        <v>236</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <f t="shared" si="4"/>
+        <v>62</v>
+      </c>
+      <c r="B84" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Rule-062</v>
+      </c>
+      <c r="C84" t="s">
+        <v>356</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <f t="shared" si="4"/>
+        <v>63</v>
+      </c>
+      <c r="B85" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Rule-063</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <f t="shared" si="4"/>
+        <v>64</v>
+      </c>
+      <c r="B86" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Rule-064</v>
+      </c>
+      <c r="C86" t="s">
+        <v>239</v>
+      </c>
+      <c r="D86" t="s">
+        <v>379</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <f t="shared" si="4"/>
+        <v>65</v>
+      </c>
+      <c r="B87" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Rule-065</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <f t="shared" si="4"/>
+        <v>66</v>
+      </c>
+      <c r="B88" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Rule-066</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <f t="shared" si="4"/>
+        <v>67</v>
+      </c>
+      <c r="B89" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Rule-067</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <f t="shared" si="4"/>
         <v>68</v>
       </c>
-      <c r="B69" s="1" t="str">
+      <c r="B90" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Rule-068</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D69" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
-        <f t="shared" si="5"/>
+      <c r="C90" t="s">
+        <v>326</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <f t="shared" si="4"/>
         <v>69</v>
       </c>
-      <c r="B70" s="1" t="str">
+      <c r="B91" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Rule-069</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D70" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
-        <f t="shared" si="5"/>
+      <c r="C91" t="s">
+        <v>327</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
-      <c r="B71" s="1" t="str">
+      <c r="B92" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Rule-070</v>
       </c>
-      <c r="C71" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D71" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
-        <f t="shared" si="5"/>
+      <c r="C92" t="s">
+        <v>384</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <f t="shared" si="4"/>
         <v>71</v>
       </c>
-      <c r="B72" s="1" t="str">
+      <c r="B93" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Rule-071</v>
       </c>
-      <c r="D72" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
-        <f t="shared" si="5"/>
+      <c r="C93" t="s">
+        <v>241</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <f t="shared" si="4"/>
         <v>72</v>
       </c>
-      <c r="B73" s="1" t="str">
+      <c r="B94" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Rule-072</v>
       </c>
-      <c r="D73" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
-        <f t="shared" si="5"/>
+      <c r="C94" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <f t="shared" si="4"/>
         <v>73</v>
       </c>
-      <c r="B74" s="1" t="str">
+      <c r="B95" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Rule-073</v>
       </c>
-      <c r="D74" t="s">
-        <v>311</v>
-      </c>
-      <c r="G74" s="1"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="1">
-        <f t="shared" si="5"/>
+      <c r="C95" t="s">
+        <v>387</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <f t="shared" si="4"/>
         <v>74</v>
       </c>
-      <c r="B75" s="1" t="str">
+      <c r="B96" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Rule-074</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D75" t="s">
-        <v>312</v>
-      </c>
-      <c r="G75" s="1"/>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
-        <f t="shared" si="5"/>
+      <c r="C96" t="s">
+        <v>389</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <f t="shared" si="4"/>
         <v>75</v>
       </c>
-      <c r="B76" s="1" t="str">
+      <c r="B97" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Rule-075</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D76" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
-        <f t="shared" si="5"/>
+      <c r="C97" t="s">
+        <v>391</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <f t="shared" si="4"/>
         <v>76</v>
       </c>
-      <c r="B77" s="1" t="str">
+      <c r="B98" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Rule-076</v>
       </c>
-      <c r="C77" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D77" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="1">
-        <f t="shared" si="5"/>
+      <c r="C98" t="s">
+        <v>393</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <f t="shared" si="4"/>
         <v>77</v>
       </c>
-      <c r="B78" s="1" t="str">
+      <c r="B99" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Rule-077</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D78" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
-        <f t="shared" si="5"/>
+      <c r="C99" t="s">
+        <v>395</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <f t="shared" si="4"/>
         <v>78</v>
       </c>
-      <c r="B79" s="1" t="str">
+      <c r="B100" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Rule-078</v>
       </c>
-      <c r="C79" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D79" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="1">
-        <f t="shared" ref="A80:A120" si="7">A79+1</f>
+      <c r="C100" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <f t="shared" si="4"/>
         <v>79</v>
       </c>
-      <c r="B80" s="1" t="str">
+      <c r="B101" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Rule-079</v>
       </c>
-      <c r="C80" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D80" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="1">
-        <f t="shared" si="7"/>
+      <c r="C101" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <f t="shared" si="4"/>
         <v>80</v>
       </c>
-      <c r="B81" s="1" t="str">
+      <c r="B102" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Rule-080</v>
       </c>
-      <c r="C81" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="1">
+      <c r="C102" t="s">
+        <v>398</v>
+      </c>
+      <c r="D102" t="s">
+        <v>399</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <f t="shared" si="4"/>
+        <v>81</v>
+      </c>
+      <c r="B103" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Rule-081</v>
+      </c>
+      <c r="C103" t="s">
+        <v>362</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <f t="shared" si="4"/>
+        <v>82</v>
+      </c>
+      <c r="B104" s="1" t="str">
+        <f t="shared" ref="B104:B113" si="7">CONCATENATE("Rule-",TEXT(A104,"000"))</f>
+        <v>Rule-082</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <f t="shared" si="4"/>
+        <v>83</v>
+      </c>
+      <c r="B105" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>81</v>
-      </c>
-      <c r="B82" s="1" t="str">
-        <f t="shared" ref="B82:B103" si="8">CONCATENATE("Rule-",TEXT(A82,"000"))</f>
-        <v>Rule-081</v>
-      </c>
-      <c r="D82" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="1">
+        <v>Rule-083</v>
+      </c>
+      <c r="C105" t="s">
+        <v>364</v>
+      </c>
+      <c r="D105" t="s">
+        <v>402</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <f t="shared" si="4"/>
+        <v>84</v>
+      </c>
+      <c r="B106" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>82</v>
-      </c>
-      <c r="B83" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>Rule-082</v>
-      </c>
-      <c r="C83" t="s">
-        <v>236</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="F83" s="1" t="s">
+        <v>Rule-084</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="D106" t="s">
+        <v>404</v>
+      </c>
+      <c r="F106" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="1">
+    <row r="107" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <f t="shared" si="4"/>
+        <v>85</v>
+      </c>
+      <c r="B107" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>83</v>
-      </c>
-      <c r="B84" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>Rule-083</v>
-      </c>
-      <c r="C84" t="s">
-        <v>356</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="F84" s="1" t="s">
+        <v>Rule-085</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="F107" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="1">
+    <row r="108" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
+        <f t="shared" si="4"/>
+        <v>86</v>
+      </c>
+      <c r="B108" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>84</v>
-      </c>
-      <c r="B85" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>Rule-084</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="F85" s="1" t="s">
+        <v>Rule-086</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F108" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="1">
+    <row r="109" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <f t="shared" si="4"/>
+        <v>87</v>
+      </c>
+      <c r="B109" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>85</v>
-      </c>
-      <c r="B86" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>Rule-085</v>
-      </c>
-      <c r="C86" t="s">
-        <v>239</v>
-      </c>
-      <c r="D86" t="s">
-        <v>379</v>
-      </c>
-      <c r="F86" s="1" t="s">
+        <v>Rule-087</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F109" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="1">
+    <row r="110" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <f t="shared" si="4"/>
+        <v>88</v>
+      </c>
+      <c r="B110" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>86</v>
-      </c>
-      <c r="B87" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>Rule-086</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="F87" s="1" t="s">
+        <v>Rule-088</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="F110" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="88" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="1">
+    <row r="111" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <f t="shared" si="4"/>
+        <v>89</v>
+      </c>
+      <c r="B111" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>87</v>
-      </c>
-      <c r="B88" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>Rule-087</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="F88" s="1" t="s">
+        <v>Rule-089</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="F111" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="89" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="1">
+    <row r="112" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
+        <f t="shared" si="4"/>
+        <v>90</v>
+      </c>
+      <c r="B112" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>88</v>
-      </c>
-      <c r="B89" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>Rule-088</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="F89" s="1" t="s">
+        <v>Rule-090</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="F112" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="1">
+    <row r="113" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
+        <f t="shared" si="4"/>
+        <v>91</v>
+      </c>
+      <c r="B113" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>89</v>
-      </c>
-      <c r="B90" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>Rule-089</v>
-      </c>
-      <c r="C90" t="s">
-        <v>326</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="F90" s="1" t="s">
+        <v>Rule-091</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="F113" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="1">
-        <f t="shared" si="7"/>
-        <v>90</v>
-      </c>
-      <c r="B91" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>Rule-090</v>
-      </c>
-      <c r="C91" t="s">
-        <v>327</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="F91" s="1" t="s">
+    <row r="114" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <f t="shared" si="4"/>
+        <v>92</v>
+      </c>
+      <c r="B114" s="1" t="str">
+        <f t="shared" ref="B114:B120" si="8">CONCATENATE("Rule-",TEXT(A114,"000"))</f>
+        <v>Rule-092</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="F114" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="1">
-        <f t="shared" si="7"/>
-        <v>91</v>
-      </c>
-      <c r="B92" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>Rule-091</v>
-      </c>
-      <c r="C92" t="s">
-        <v>384</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="1">
-        <f t="shared" si="7"/>
-        <v>92</v>
-      </c>
-      <c r="B93" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>Rule-092</v>
-      </c>
-      <c r="C93" t="s">
-        <v>241</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="1">
-        <f t="shared" si="7"/>
+    <row r="115" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <f t="shared" si="4"/>
         <v>93</v>
       </c>
-      <c r="B94" s="1" t="str">
+      <c r="B115" s="1" t="str">
         <f t="shared" si="8"/>
         <v>Rule-093</v>
       </c>
-      <c r="C94" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="F94" s="1" t="s">
+      <c r="C115" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="F115" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="1">
-        <f t="shared" si="7"/>
+    <row r="116" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="1">
+        <f t="shared" si="4"/>
         <v>94</v>
       </c>
-      <c r="B95" s="1" t="str">
+      <c r="B116" s="1" t="str">
         <f t="shared" si="8"/>
         <v>Rule-094</v>
       </c>
-      <c r="C95" t="s">
-        <v>387</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="F95" s="1" t="s">
+      <c r="C116" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="F116" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="1">
-        <f t="shared" si="7"/>
+    <row r="117" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="1">
+        <f t="shared" si="4"/>
         <v>95</v>
       </c>
-      <c r="B96" s="1" t="str">
+      <c r="B117" s="1" t="str">
         <f t="shared" si="8"/>
         <v>Rule-095</v>
       </c>
-      <c r="C96" t="s">
-        <v>389</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="F96" s="1" t="s">
+      <c r="C117" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="F117" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="1">
-        <f t="shared" si="7"/>
+    <row r="118" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="1">
+        <f t="shared" si="4"/>
         <v>96</v>
       </c>
-      <c r="B97" s="1" t="str">
+      <c r="B118" s="1" t="str">
         <f t="shared" si="8"/>
         <v>Rule-096</v>
       </c>
-      <c r="C97" t="s">
-        <v>391</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="F97" s="1" t="s">
+      <c r="C118" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="F118" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="1">
-        <f t="shared" si="7"/>
+    <row r="119" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
+        <f t="shared" si="4"/>
         <v>97</v>
       </c>
-      <c r="B98" s="1" t="str">
+      <c r="B119" s="1" t="str">
         <f t="shared" si="8"/>
         <v>Rule-097</v>
       </c>
-      <c r="C98" t="s">
-        <v>393</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="F98" s="1" t="s">
+      <c r="C119" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="F119" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="1">
-        <f t="shared" si="7"/>
+    <row r="120" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
+        <f t="shared" si="4"/>
         <v>98</v>
       </c>
-      <c r="B99" s="1" t="str">
+      <c r="B120" s="1" t="str">
         <f t="shared" si="8"/>
         <v>Rule-098</v>
-      </c>
-      <c r="C99" t="s">
-        <v>395</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="F99" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="1">
-        <f t="shared" si="7"/>
-        <v>99</v>
-      </c>
-      <c r="B100" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>Rule-099</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="1">
-        <f t="shared" si="7"/>
-        <v>100</v>
-      </c>
-      <c r="B101" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>Rule-100</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="F101" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="1">
-        <f t="shared" si="7"/>
-        <v>101</v>
-      </c>
-      <c r="B102" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>Rule-101</v>
-      </c>
-      <c r="C102" t="s">
-        <v>398</v>
-      </c>
-      <c r="D102" t="s">
-        <v>399</v>
-      </c>
-      <c r="F102" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="1">
-        <f t="shared" si="7"/>
-        <v>102</v>
-      </c>
-      <c r="B103" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>Rule-102</v>
-      </c>
-      <c r="C103" t="s">
-        <v>362</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="F103" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="1">
-        <f t="shared" si="7"/>
-        <v>103</v>
-      </c>
-      <c r="B104" s="1" t="str">
-        <f t="shared" ref="B104:B113" si="9">CONCATENATE("Rule-",TEXT(A104,"000"))</f>
-        <v>Rule-103</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="F104" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="1">
-        <f t="shared" si="7"/>
-        <v>104</v>
-      </c>
-      <c r="B105" s="1" t="str">
-        <f t="shared" si="9"/>
-        <v>Rule-104</v>
-      </c>
-      <c r="C105" t="s">
-        <v>364</v>
-      </c>
-      <c r="D105" t="s">
-        <v>402</v>
-      </c>
-      <c r="F105" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="1">
-        <f t="shared" si="7"/>
-        <v>105</v>
-      </c>
-      <c r="B106" s="1" t="str">
-        <f t="shared" si="9"/>
-        <v>Rule-105</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="D106" t="s">
-        <v>404</v>
-      </c>
-      <c r="F106" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="1">
-        <f t="shared" si="7"/>
-        <v>106</v>
-      </c>
-      <c r="B107" s="1" t="str">
-        <f t="shared" si="9"/>
-        <v>Rule-106</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="F107" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="1">
-        <f t="shared" si="7"/>
-        <v>107</v>
-      </c>
-      <c r="B108" s="1" t="str">
-        <f t="shared" si="9"/>
-        <v>Rule-107</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="F108" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="1">
-        <f t="shared" si="7"/>
-        <v>108</v>
-      </c>
-      <c r="B109" s="1" t="str">
-        <f t="shared" si="9"/>
-        <v>Rule-108</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="F109" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="1">
-        <f t="shared" si="7"/>
-        <v>109</v>
-      </c>
-      <c r="B110" s="1" t="str">
-        <f t="shared" si="9"/>
-        <v>Rule-109</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="F110" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="1">
-        <f t="shared" si="7"/>
-        <v>110</v>
-      </c>
-      <c r="B111" s="1" t="str">
-        <f t="shared" si="9"/>
-        <v>Rule-110</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="F111" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="1">
-        <f t="shared" si="7"/>
-        <v>111</v>
-      </c>
-      <c r="B112" s="1" t="str">
-        <f t="shared" si="9"/>
-        <v>Rule-111</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="F112" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="1">
-        <f t="shared" si="7"/>
-        <v>112</v>
-      </c>
-      <c r="B113" s="1" t="str">
-        <f t="shared" si="9"/>
-        <v>Rule-112</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="F113" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="1">
-        <f t="shared" si="7"/>
-        <v>113</v>
-      </c>
-      <c r="B114" s="1" t="str">
-        <f t="shared" ref="B114:B120" si="10">CONCATENATE("Rule-",TEXT(A114,"000"))</f>
-        <v>Rule-113</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="F114" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="1">
-        <f t="shared" si="7"/>
-        <v>114</v>
-      </c>
-      <c r="B115" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v>Rule-114</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="1">
-        <f t="shared" si="7"/>
-        <v>115</v>
-      </c>
-      <c r="B116" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v>Rule-115</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="F116" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="1">
-        <f t="shared" si="7"/>
-        <v>116</v>
-      </c>
-      <c r="B117" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v>Rule-116</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="F117" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="1">
-        <f t="shared" si="7"/>
-        <v>117</v>
-      </c>
-      <c r="B118" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v>Rule-117</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="F118" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="1">
-        <f t="shared" si="7"/>
-        <v>118</v>
-      </c>
-      <c r="B119" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v>Rule-118</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="F119" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="1">
-        <f t="shared" si="7"/>
-        <v>119</v>
-      </c>
-      <c r="B120" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v>Rule-119</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>248</v>
@@ -3961,11 +4546,17 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A3:B1000">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND(A3&lt;&gt;"",A3=A2)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E98"/>
   <sheetViews>
@@ -5437,7 +6028,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C86"/>
   <sheetViews>

</xml_diff>

<commit_message>
* Added "security" to "securing-your-site" to urlmapping * Added release notes to product versions and used it in what's new.
</commit_message>
<xml_diff>
--- a/_build/urlmap/DC-URLmapping.xlsx
+++ b/_build/urlmap/DC-URLmapping.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="420">
   <si>
     <t>DNN8-Requirements.html</t>
   </si>
@@ -1271,6 +1271,12 @@
   </si>
   <si>
     <t>new</t>
+  </si>
+  <si>
+    <t>security</t>
+  </si>
+  <si>
+    <t>securing-your-site</t>
   </si>
 </sst>
 </file>
@@ -1669,10 +1675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62:B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2197,6 +2203,14 @@
       </c>
       <c r="C61" s="1" t="s">
         <v>235</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>419</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* Removed the hyphens in the breadcrumbs. * Renamed "security" folder and "security.dita" to "securing-your-site" and "securing-your-site.dita", respectively. Updated web.config-producing files and ditamaps. * Added Evoq Social release notes to existing files. * Added short blurb to about-structured-content.dita.
</commit_message>
<xml_diff>
--- a/_build/urlmap/DC-URLmapping.xlsx
+++ b/_build/urlmap/DC-URLmapping.xlsx
@@ -12,12 +12,12 @@
     <sheet name="20160323 old2new" sheetId="2" r:id="rId3"/>
     <sheet name="20160309 old2new" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="422">
   <si>
     <t>DNN8-Requirements.html</t>
   </si>
@@ -1277,6 +1277,12 @@
   </si>
   <si>
     <t>securing-your-site</t>
+  </si>
+  <si>
+    <t>security/security.html</t>
+  </si>
+  <si>
+    <t>securing-your-site/securing-your-site.html</t>
   </si>
 </sst>
 </file>
@@ -1675,10 +1681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62:B62"/>
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2211,6 +2217,14 @@
       </c>
       <c r="B62" s="1" t="s">
         <v>419</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>421</v>
       </c>
     </row>
   </sheetData>

</xml_diff>